<commit_message>
prototype hotspot investigate modal, more hookups, testing content (not tested yet)
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783695B9-5982-412C-9B86-2EF00245CF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1590E608-4B21-4CE8-AB9E-821A10005F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5670" yWindow="1665" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Key</t>
   </si>
@@ -40,18 +40,6 @@
     <t>credits_desc</t>
   </si>
   <si>
-    <t>ready</t>
-  </si>
-  <si>
-    <t>READY</t>
-  </si>
-  <si>
-    <t>go</t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
     <t>options</t>
   </si>
   <si>
@@ -98,6 +86,66 @@
   </si>
   <si>
     <t>Project Bloom: A Quest for Home</t>
+  </si>
+  <si>
+    <t>season_winter</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>season_spring</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>season_summer</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>season_autumn</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>atmosphere_altitude</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
+  <si>
+    <t>atmosphere_humidity</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>atmosphere_temperature</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>atmosphere_windStrength</t>
+  </si>
+  <si>
+    <t>Wind Strength</t>
+  </si>
+  <si>
+    <t>climate_temperate</t>
+  </si>
+  <si>
+    <t>Temperate</t>
+  </si>
+  <si>
+    <t>region_NA</t>
+  </si>
+  <si>
+    <t>North American Great Plains</t>
   </si>
 </sst>
 </file>
@@ -433,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -474,79 +522,143 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaks to hotspot inspection, testing confirmed
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1590E608-4B21-4CE8-AB9E-821A10005F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254F4451-B9C9-4A8C-B9F4-7CA4458C240B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5670" yWindow="1665" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Key</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>North American Great Plains</t>
+  </si>
+  <si>
+    <t>climate_title</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>region_title</t>
+  </si>
+  <si>
+    <t>Region</t>
   </si>
 </sst>
 </file>
@@ -481,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,17 +659,33 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
overworld modal art, moved stuff around, refactor hotspot data, some consideration on overworld gameflow.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254F4451-B9C9-4A8C-B9F4-7CA4458C240B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914753E3-6A09-4A55-9022-171A5FE0BA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="1665" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Key</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>criteria</t>
+  </si>
+  <si>
+    <t>CRITERIA</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,97 +601,105 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modal atmosphere analyze for hotspot, changes to data for better tweaking
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914753E3-6A09-4A55-9022-171A5FE0BA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FC16AF-A2CA-490D-B7B3-B0A52D2FBD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Key</t>
   </si>
@@ -164,6 +164,36 @@
   </si>
   <si>
     <t>CRITERIA</t>
+  </si>
+  <si>
+    <t>hotspotAnalyze_title</t>
+  </si>
+  <si>
+    <t>investigate</t>
+  </si>
+  <si>
+    <t>INVESTIGATE</t>
+  </si>
+  <si>
+    <t>Atmospheric Reading</t>
+  </si>
+  <si>
+    <t>season_title</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>analyzing</t>
+  </si>
+  <si>
+    <t>ANALYZING</t>
+  </si>
+  <si>
+    <t>incompatible</t>
+  </si>
+  <si>
+    <t>INCOMPATIBLE!</t>
   </si>
 </sst>
 </file>
@@ -499,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,97 +639,137 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modal investigate art/tweaks, critic panel art/animations
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FC16AF-A2CA-490D-B7B3-B0A52D2FBD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2E7D9D-89D1-43AE-8126-B65CF0390678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Key</t>
   </si>
@@ -194,6 +194,18 @@
   </si>
   <si>
     <t>INCOMPATIBLE!</t>
+  </si>
+  <si>
+    <t>launch</t>
+  </si>
+  <si>
+    <t>LAUNCH</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>BACK</t>
   </si>
 </sst>
 </file>
@@ -529,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,105 +683,121 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
weather forecast modal layout/art
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2E7D9D-89D1-43AE-8126-B65CF0390678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CB745B-65C5-4324-A1A7-77EBD337FC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Key</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>BACK</t>
+  </si>
+  <si>
+    <t>weatherForecast</t>
+  </si>
+  <si>
+    <t>Weather Forecast</t>
   </si>
 </sst>
 </file>
@@ -541,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,6 +807,14 @@
         <v>41</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
implement logic for ModalWeatherForecast (untested)
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CB745B-65C5-4324-A1A7-77EBD337FC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0489FD9C-E514-4A06-9E3B-7AAC6C538F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Key</t>
   </si>
@@ -212,6 +212,54 @@
   </si>
   <si>
     <t>Weather Forecast</t>
+  </si>
+  <si>
+    <t>day_today</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>day_monday</t>
+  </si>
+  <si>
+    <t>day_tuesday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>day_wednesday</t>
+  </si>
+  <si>
+    <t>day_thursday</t>
+  </si>
+  <si>
+    <t>day_friday</t>
+  </si>
+  <si>
+    <t>day_saturday</t>
+  </si>
+  <si>
+    <t>day_sunday</t>
   </si>
 </sst>
 </file>
@@ -547,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,6 +863,70 @@
         <v>63</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
more colony hud art/animation/layout
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0489FD9C-E514-4A06-9E3B-7AAC6C538F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD15B5B1-C4D4-45AB-AB48-117BC834C433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Key</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>day_sunday</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>CANCEL</t>
   </si>
 </sst>
 </file>
@@ -595,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,177 +759,185 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
a bunch of adjustments to logic, bug fixes, tweak level 1 flow (without enemies), pause game if house is available.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD15B5B1-C4D4-45AB-AB48-117BC834C433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67824061-89DE-4F71-801E-5BBEFDA7B151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Key</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>CANCEL</t>
+  </si>
+  <si>
+    <t>new_house</t>
+  </si>
+  <si>
+    <t>New house available! Deploy it to continue.</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,177 +773,185 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
victory stuff, more data tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67824061-89DE-4F71-801E-5BBEFDA7B151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821E400D-71AF-4317-BDD6-E59834F56524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Key</t>
   </si>
@@ -271,7 +271,25 @@
     <t>new_house</t>
   </si>
   <si>
-    <t>New house available! Deploy it to continue.</t>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>houses_deployed</t>
+  </si>
+  <si>
+    <t>Homes Deployed</t>
+  </si>
+  <si>
+    <t>A new house is available! Deploy it to progress.</t>
   </si>
 </sst>
 </file>
@@ -607,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,182 +794,206 @@
         <v>82</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
background stuff for level 1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821E400D-71AF-4317-BDD6-E59834F56524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F19C3C-F204-4813-B711-46A3D8551037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Key</t>
   </si>
@@ -290,6 +290,36 @@
   </si>
   <si>
     <t>A new house is available! Deploy it to progress.</t>
+  </si>
+  <si>
+    <t>weather_sunny</t>
+  </si>
+  <si>
+    <t>Sunny</t>
+  </si>
+  <si>
+    <t>weather_partly_sunny</t>
+  </si>
+  <si>
+    <t>Partly Sunny</t>
+  </si>
+  <si>
+    <t>weather_mostly_cloudy</t>
+  </si>
+  <si>
+    <t>Mostly Cloudy</t>
+  </si>
+  <si>
+    <t>weather_light_rain</t>
+  </si>
+  <si>
+    <t>Light Rain</t>
+  </si>
+  <si>
+    <t>weather_rain</t>
+  </si>
+  <si>
+    <t>Rain</t>
   </si>
 </sst>
 </file>
@@ -625,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,6 +1027,46 @@
         <v>74</v>
       </c>
     </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
implement colony sequence control for tutorial and lessons, added enemies to level 1.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F19C3C-F204-4813-B711-46A3D8551037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B132F4E6-531E-4428-87AA-3A9F5C4C1475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7005" yWindow="2205" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="2670" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Key</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>Rain</t>
+  </si>
+  <si>
+    <t>weather_cloudy</t>
+  </si>
+  <si>
+    <t>Cloudy</t>
   </si>
 </sst>
 </file>
@@ -655,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,6 +1073,14 @@
         <v>99</v>
       </c>
     </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
initial level 2 stuff, implemented hazard protocols
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B132F4E6-531E-4428-87AA-3A9F5C4C1475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F643CE-74CD-43B9-AEC1-2D590A4C8473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="2670" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Key</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>Cloudy</t>
+  </si>
+  <si>
+    <t>weather_typhoon</t>
+  </si>
+  <si>
+    <t>Typhoon</t>
   </si>
 </sst>
 </file>
@@ -661,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,6 +1087,14 @@
         <v>101</v>
       </c>
     </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
level 2 weather stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F643CE-74CD-43B9-AEC1-2D590A4C8473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0111AFA-5C40-4D56-BBFF-C936E61684E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="2670" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Key</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>Typhoon</t>
+  </si>
+  <si>
+    <t>weather_heavy_rain</t>
+  </si>
+  <si>
+    <t>Heavy Rain</t>
   </si>
 </sst>
 </file>
@@ -667,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,33 +1071,41 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
colony 3 stuff: background, weather, sequence, etc. (still need enemy spawns)
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0111AFA-5C40-4D56-BBFF-C936E61684E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F964507-B759-4211-B5E2-B7C978315F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="2670" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>Key</t>
   </si>
@@ -338,6 +338,18 @@
   </si>
   <si>
     <t>Heavy Rain</t>
+  </si>
+  <si>
+    <t>weather_haze</t>
+  </si>
+  <si>
+    <t>Haze</t>
+  </si>
+  <si>
+    <t>weather_dustStorm</t>
+  </si>
+  <si>
+    <t>Dust Storm</t>
   </si>
 </sst>
 </file>
@@ -673,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,6 +1121,22 @@
         <v>103</v>
       </c>
     </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
overworld stuff, more ui art
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441E7874-2C81-451D-9636-8935A67EE62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9977D5-AA62-425F-86D9-5F4ECC2DC9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="2670" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>Key</t>
   </si>
@@ -362,6 +362,96 @@
   </si>
   <si>
     <t>Snow</t>
+  </si>
+  <si>
+    <t>region_PH</t>
+  </si>
+  <si>
+    <t>climate_tropical</t>
+  </si>
+  <si>
+    <t>Tropical</t>
+  </si>
+  <si>
+    <t>region_GB</t>
+  </si>
+  <si>
+    <t>British Isles</t>
+  </si>
+  <si>
+    <t>climate_oceanic</t>
+  </si>
+  <si>
+    <t>Oceanic</t>
+  </si>
+  <si>
+    <t>region_MG</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>region_EG</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>climate_desert</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>region_GL</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>climate_tundra</t>
+  </si>
+  <si>
+    <t>Tundra</t>
+  </si>
+  <si>
+    <t>region_BR</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>region_CL</t>
+  </si>
+  <si>
+    <t>Northern Luzon, Philippines</t>
+  </si>
+  <si>
+    <t>Andes Mountains, Chile</t>
+  </si>
+  <si>
+    <t>climate_highland</t>
+  </si>
+  <si>
+    <t>Highland</t>
+  </si>
+  <si>
+    <t>climate_mediterranean</t>
+  </si>
+  <si>
+    <t>Mediterranean</t>
+  </si>
+  <si>
+    <t>region_IT</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>region_AU</t>
+  </si>
+  <si>
+    <t>Australian Outback</t>
   </si>
 </sst>
 </file>
@@ -697,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,185 +1073,305 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>78</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>106</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start scene, initial intro, frog icons
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9977D5-AA62-425F-86D9-5F4ECC2DC9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE1CCC-870A-4CFA-8E0C-D3FE0821937F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="2670" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35655" yWindow="2355" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>Key</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Made by: RENEGADEWARE</t>
   </si>
   <si>
-    <t>Project Bloom: A Quest for Home</t>
-  </si>
-  <si>
     <t>season_winter</t>
   </si>
   <si>
@@ -452,6 +449,69 @@
   </si>
   <si>
     <t>Australian Outback</t>
+  </si>
+  <si>
+    <t>Project Bloom\n&lt;size=30&gt;A Quest for Home&lt;/size&gt;</t>
+  </si>
+  <si>
+    <t>newGame</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>Unidentified ships approaching Earth!</t>
+  </si>
+  <si>
+    <t>That’s better! Let’s see if they are of any threat…</t>
+  </si>
+  <si>
+    <t>intro_0_0</t>
+  </si>
+  <si>
+    <t>intro_1_0</t>
+  </si>
+  <si>
+    <t>intro_2_0</t>
+  </si>
+  <si>
+    <t>intro_3_0</t>
+  </si>
+  <si>
+    <t>intro_3_1</t>
+  </si>
+  <si>
+    <t>intro_4_0</t>
+  </si>
+  <si>
+    <t>intro_4_1</t>
+  </si>
+  <si>
+    <t>intro_4_2</t>
+  </si>
+  <si>
+    <t>They appear to be frog-like. Let me put on my frog suit to communicate with these peculiar creatures!</t>
+  </si>
+  <si>
+    <t>Well, we can’t just let them hang about in space. Besides, how often are we visited by sentient aliens from outer space?</t>
+  </si>
+  <si>
+    <t>It looks like they have been exiled from their planet, and are looking for a new home.</t>
+  </si>
+  <si>
+    <t>They are expressing their gratitude, and are ready to cooperate in exchange for their refuge.</t>
+  </si>
+  <si>
+    <t>Well, why not? Let’s give these hapless frogs some proper homes to settle in. There’s still plenty of room here on Earth.</t>
+  </si>
+  <si>
+    <t>Now commencing operation: Project Bloom – A quest for home!</t>
   </si>
 </sst>
 </file>
@@ -501,11 +561,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +883,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,490 +952,570 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>120</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>135</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>65</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>111</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>113</v>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>153</v>
+      </c>
+      <c r="B77" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overworld 1 lesson and tutorial
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE1CCC-870A-4CFA-8E0C-D3FE0821937F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D89F56E-751B-4BCB-89C8-E7DF7606196D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35655" yWindow="2355" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42090" yWindow="645" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
   <si>
     <t>Key</t>
   </si>
@@ -512,6 +512,126 @@
   </si>
   <si>
     <t>Now commencing operation: Project Bloom – A quest for home!</t>
+  </si>
+  <si>
+    <t>sunIllustrate_title</t>
+  </si>
+  <si>
+    <t>Sunlight Direction</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>sunIllustrate_hot</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>sunIllustrate_warm</t>
+  </si>
+  <si>
+    <t>Warm</t>
+  </si>
+  <si>
+    <t>overworld_1_intro_0</t>
+  </si>
+  <si>
+    <t>This is the map of Earth. The frogs are very particular with their choice of habitat.</t>
+  </si>
+  <si>
+    <t>overworld_1_intro_1</t>
+  </si>
+  <si>
+    <t>We’ll need to determine where to place the frogs by looking at their criteria.</t>
+  </si>
+  <si>
+    <t>overworld_1_criteria_0</t>
+  </si>
+  <si>
+    <t>In this case, we need to find a place where it’s fairly warm and humid.</t>
+  </si>
+  <si>
+    <t>overworld_1_hud_0</t>
+  </si>
+  <si>
+    <t>Now let’s view the temperature readings of Earth.</t>
+  </si>
+  <si>
+    <t>overworld_1_hud_1</t>
+  </si>
+  <si>
+    <t>overworld_1_temp_0</t>
+  </si>
+  <si>
+    <t>As you can see, the temperature is consistently hot starting from the equator, and gets colder further north or south.</t>
+  </si>
+  <si>
+    <t>overworld_1_humid_0</t>
+  </si>
+  <si>
+    <t>Next is the humidity readings of Earth. The percentage tells us how much water vapor is present on air.</t>
+  </si>
+  <si>
+    <t>overworld_1_humid_1</t>
+  </si>
+  <si>
+    <t>Notice how humidity tends to be higher in large forest and jungle areas, such as the Amazon rainforest.</t>
+  </si>
+  <si>
+    <t>Now go ahead and find a place for the frogs to land. Simply click around the map to find the spot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remember to make use of the temperature and humidity reading. </t>
+  </si>
+  <si>
+    <t>overworld_1_hotspot_0</t>
+  </si>
+  <si>
+    <t>overworld_1_hotspot_1</t>
+  </si>
+  <si>
+    <t>overworld_1_hotspot_2</t>
+  </si>
+  <si>
+    <t>overworld_1_analyze_0</t>
+  </si>
+  <si>
+    <t>overworld_1_analyze_1</t>
+  </si>
+  <si>
+    <t>overworld_1_analyze_2</t>
+  </si>
+  <si>
+    <t>Since the earth rotate at a slightly tilted axis around the sun, the atmosphere can change throughout the year.</t>
+  </si>
+  <si>
+    <t>Why don’t we adjust the time by selecting a different season.</t>
+  </si>
+  <si>
+    <t>overworld_1_investigate_0</t>
+  </si>
+  <si>
+    <t>Now you just need to pick a particular location on the land for the frogs.</t>
+  </si>
+  <si>
+    <t>When the majority of the frogs approve, we can finally launch the expedition!</t>
+  </si>
+  <si>
+    <t>overworld_1_investigate_1</t>
+  </si>
+  <si>
+    <t>On the lefthand side of the map are the latitude values. This is the angular distance relative to the earth’s equator (middle of the map).</t>
+  </si>
+  <si>
+    <t>Hint: we are looking for a temperate climate, perhaps somewhere in North America...</t>
+  </si>
+  <si>
+    <t>Looks like the temperature is too low. We will need to change the time of the year to land on this spot.</t>
   </si>
 </sst>
 </file>
@@ -850,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,458 +1184,618 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>133</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>150</v>
-      </c>
-      <c r="B74" t="s">
-        <v>148</v>
+        <v>111</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B75" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B78" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B79" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>156</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
+      </c>
+      <c r="B80" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>157</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>174</v>
+      </c>
+      <c r="B87" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>178</v>
+      </c>
+      <c r="B89" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>180</v>
+      </c>
+      <c r="B90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>181</v>
+      </c>
+      <c r="B91" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>185</v>
+      </c>
+      <c r="B93" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>191</v>
+      </c>
+      <c r="B96" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>197</v>
+      </c>
+      <c r="B100" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dialogs for the rest of overworld and colony
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ABD6D6-88F5-4B58-98E4-0276948C066A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1695827-D6E6-4B94-91ED-23A3184F408C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="1860" windowWidth="28365" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41025" yWindow="1095" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="354">
   <si>
     <t>Key</t>
   </si>
@@ -800,6 +800,288 @@
   </si>
   <si>
     <t>A mole! These creatures don’t see very well, so they mistake our structures as something to dig through.</t>
+  </si>
+  <si>
+    <t>overworld_2_intro_0</t>
+  </si>
+  <si>
+    <t>overworld_2_intro_1</t>
+  </si>
+  <si>
+    <t>In that case, we’ll need to check the wind readings of Earth.</t>
+  </si>
+  <si>
+    <t>overworld_2_wind_0</t>
+  </si>
+  <si>
+    <t>overworld_2_wind_temp_0</t>
+  </si>
+  <si>
+    <t>overworld_2_wind_temp_1</t>
+  </si>
+  <si>
+    <t>overworld_2_wind_temp_2</t>
+  </si>
+  <si>
+    <t>This cycle continues as the wind travels, building up more speed along the way.</t>
+  </si>
+  <si>
+    <t>overworld_2_post_intro_0</t>
+  </si>
+  <si>
+    <t>overworld_2_post_intro_1</t>
+  </si>
+  <si>
+    <t>overworld_2_post_intro_2</t>
+  </si>
+  <si>
+    <t>Anyhow, let’s find places where the wind might by strong. Try looking for areas prone to hurricanes along coastal regions.</t>
+  </si>
+  <si>
+    <t>Remember to check the different seasons to see how the wind changes to various positions across Earth.</t>
+  </si>
+  <si>
+    <t>This time around, there are more than one hotspot to discover on the map. Only one of them is will match with the frogs’ criteria.</t>
+  </si>
+  <si>
+    <t>Our next batch of frogs are keen on living in a windy environment, as well as hot and humid.</t>
+  </si>
+  <si>
+    <t>Notice the winds forming into a swirly motion? These are tropical cyclones, sometimes referred to as: hurricanes, or typhoons.</t>
+  </si>
+  <si>
+    <t>As you can see, the warm energy from the ocean rises, forming low pressure from below. This causes more air to fill in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The air filling in must then rise because of the heat, accumulating water which release more heat. </t>
+  </si>
+  <si>
+    <t>colony_2_intro_0</t>
+  </si>
+  <si>
+    <t>colony_2_intro_1</t>
+  </si>
+  <si>
+    <t>colony_2_intro_2</t>
+  </si>
+  <si>
+    <t>Looks like we’ve landed in a tropical climate. Where it’s hot and humid all year round with plenty of rain.</t>
+  </si>
+  <si>
+    <t>Though it looks like we’re getting more rain than usual, something is afoot...</t>
+  </si>
+  <si>
+    <t>Perhaps we should take a careful look at the weather forecast.</t>
+  </si>
+  <si>
+    <t>colony_2_mushroom_0</t>
+  </si>
+  <si>
+    <t>colony_2_mushroom_1</t>
+  </si>
+  <si>
+    <t>colony_2_mushroom_2</t>
+  </si>
+  <si>
+    <t>Uh oh, a mushroom has grown near one of our structures!</t>
+  </si>
+  <si>
+    <t>Since there's a lot of moisture in the region, the fungi that grow these mushrooms are able to absorb a lot of nutrients.</t>
+  </si>
+  <si>
+    <t>Their spores appear to be harmful to the frogs! Make sure to have a gardener around to take care of them!</t>
+  </si>
+  <si>
+    <t>colony_2_fly_0</t>
+  </si>
+  <si>
+    <t>colony_2_fly_1</t>
+  </si>
+  <si>
+    <t>colony_2_fly_2</t>
+  </si>
+  <si>
+    <t>Look out, it's a beetle!</t>
+  </si>
+  <si>
+    <t>Due to the consistent warmth in tropical climates, insects are able to thrive throughout the year.</t>
+  </si>
+  <si>
+    <t>These troublesome insects can be dealt with by a hero frog. Make sure to have one around to rout them out.</t>
+  </si>
+  <si>
+    <t>colony_2_hazzard_0</t>
+  </si>
+  <si>
+    <t>colony_2_hazzard_1</t>
+  </si>
+  <si>
+    <t>colony_2_hazzard_2</t>
+  </si>
+  <si>
+    <t>colony_2_hazzard_3</t>
+  </si>
+  <si>
+    <t>colony_2_hazzard_4</t>
+  </si>
+  <si>
+    <t>Take cover, a hurricane is heading our way!</t>
+  </si>
+  <si>
+    <t>As mentioned before about hurricanes: the wind speed that has accumulated over low pressure from the surface has reached critical speed.</t>
+  </si>
+  <si>
+    <t>Our frogs must take cover. Fortunately, their structures are made of sturdy stuff, causing it to withstand the staggering winds!</t>
+  </si>
+  <si>
+    <t>However, along with strong winds, the water that is released from the storm will cause flood across the land.</t>
+  </si>
+  <si>
+    <t>Make certain that no important structures are within the flooding area, or they will get damaged.</t>
+  </si>
+  <si>
+    <t>overworld_3_intro_0</t>
+  </si>
+  <si>
+    <t>overworld_3_intro_1</t>
+  </si>
+  <si>
+    <t>Our next batch of frogs are looking for a warm place with low humidity, and some nice breeze.</t>
+  </si>
+  <si>
+    <t>In that case, we should look for a desert climate!</t>
+  </si>
+  <si>
+    <t>overworld_3_investigate_0</t>
+  </si>
+  <si>
+    <t>overworld_3_investigate_1</t>
+  </si>
+  <si>
+    <t>overworld_3_investigate_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Now it may seem that these frogs would want to bask in the sun all day long. </t>
+  </si>
+  <si>
+    <t>However, they will still need some water source to sustain themselves!</t>
+  </si>
+  <si>
+    <t>Look for a suitable place where there are underground waters that we can extract.</t>
+  </si>
+  <si>
+    <t>colony_3_intro_0</t>
+  </si>
+  <si>
+    <t>colony_3_intro_1</t>
+  </si>
+  <si>
+    <t>The desert climate...This dry and hot environment will leave us with little to no water for our plants.</t>
+  </si>
+  <si>
+    <t>Fortunately, there are underground waters we can extract from to make this land more habitable.</t>
+  </si>
+  <si>
+    <t>colony_3_water_0</t>
+  </si>
+  <si>
+    <t>colony_3_water_1</t>
+  </si>
+  <si>
+    <t>Since the ground here is not ideal for growing plants, we will have to do a bit of landscaping.</t>
+  </si>
+  <si>
+    <t>First, we will need to build a water tank where water is accessible.</t>
+  </si>
+  <si>
+    <t>colony_3_landscaping_0</t>
+  </si>
+  <si>
+    <t>Now that we have a water source, summon a landscaper to irrigate the land.</t>
+  </si>
+  <si>
+    <t>colony_3_landscaping_complete_0</t>
+  </si>
+  <si>
+    <t>colony_3_landscaping_complete_1</t>
+  </si>
+  <si>
+    <t>Excellent! Now that there’s an irrigated land, you can now place a plant on it. Do this now.</t>
+  </si>
+  <si>
+    <t>We can proceed onward once we have increased the population.</t>
+  </si>
+  <si>
+    <t>overworld_4_intro_0</t>
+  </si>
+  <si>
+    <t>overworld_4_intro_1</t>
+  </si>
+  <si>
+    <t>This is our final batch of frogs, and they seem eager to settle in the highlands where it’s cold and snowy.</t>
+  </si>
+  <si>
+    <t>Why don’t we look for a spot in the mountainous area.</t>
+  </si>
+  <si>
+    <t>overworld_4_investigate_0</t>
+  </si>
+  <si>
+    <t>overworld_4_investigate_1</t>
+  </si>
+  <si>
+    <t>Although we are in an area that is mostly a tropical climate, remember that altitude can also affect the climate.</t>
+  </si>
+  <si>
+    <t>Go further up where the air pressure and temperature are lower.</t>
+  </si>
+  <si>
+    <t>colony_4_intro_0</t>
+  </si>
+  <si>
+    <t>colony_4_intro_1</t>
+  </si>
+  <si>
+    <t>The highland climate is quite comfy despite the consistent cold weather. We’ll need more than usual power to keep our houses warm.</t>
+  </si>
+  <si>
+    <t>Just like in the desert climate, the ground here is not ideal for plants to grow, so landscaping will be crucial.</t>
+  </si>
+  <si>
+    <t>colony_4_landscape_0</t>
+  </si>
+  <si>
+    <t>colony_4_landscape_1</t>
+  </si>
+  <si>
+    <t>colony_4_landscape_2</t>
+  </si>
+  <si>
+    <t>Since we can’t place plants on these rigid grounds, we’ll once again need the help of landscapers to shape the land.</t>
+  </si>
+  <si>
+    <t>You won’t have to worry about where to place the water thank this time around.</t>
+  </si>
+  <si>
+    <t>We will be able to proceed once the frog population has increased.</t>
+  </si>
+  <si>
+    <t>colony_4_cave_0</t>
+  </si>
+  <si>
+    <t>colony_4_cave_1</t>
+  </si>
+  <si>
+    <t>colony_4_cave_2</t>
+  </si>
+  <si>
+    <t>Uh oh! A cave has emerged from the ground!</t>
+  </si>
+  <si>
+    <t>Critters will keep emerging from these caves so long as it remains. Fortunately, an engineer can demolish it.</t>
+  </si>
+  <si>
+    <t>Make sure to also have a hero frog around to deal with the critters, while the engineers do their work!</t>
   </si>
 </sst>
 </file>
@@ -1138,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,6 +2472,382 @@
         <v>251</v>
       </c>
     </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>260</v>
+      </c>
+      <c r="B130" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>261</v>
+      </c>
+      <c r="B131" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>263</v>
+      </c>
+      <c r="B132" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>264</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>265</v>
+      </c>
+      <c r="B134" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>266</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>268</v>
+      </c>
+      <c r="B136" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>269</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>270</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>278</v>
+      </c>
+      <c r="B139" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>279</v>
+      </c>
+      <c r="B140" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>280</v>
+      </c>
+      <c r="B141" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>284</v>
+      </c>
+      <c r="B142" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>285</v>
+      </c>
+      <c r="B143" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>286</v>
+      </c>
+      <c r="B144" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>290</v>
+      </c>
+      <c r="B145" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>291</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>292</v>
+      </c>
+      <c r="B147" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>296</v>
+      </c>
+      <c r="B148" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>297</v>
+      </c>
+      <c r="B149" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>298</v>
+      </c>
+      <c r="B150" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>299</v>
+      </c>
+      <c r="B151" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>300</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>306</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>307</v>
+      </c>
+      <c r="B154" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>310</v>
+      </c>
+      <c r="B155" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>311</v>
+      </c>
+      <c r="B156" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>316</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>317</v>
+      </c>
+      <c r="B159" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>320</v>
+      </c>
+      <c r="B160" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>321</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>324</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>326</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>327</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>330</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>331</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>334</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>335</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>338</v>
+      </c>
+      <c r="B169" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>339</v>
+      </c>
+      <c r="B170" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>342</v>
+      </c>
+      <c r="B171" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>343</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>348</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>349</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
some bug fixes, build for submission, some level tweaks, tired
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2113F607-1D2F-4B4F-AFC4-26A240D5270B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C9C9C8-33B5-4938-A981-47C1B532E38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5310" yWindow="2550" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="364">
   <si>
     <t>Key</t>
   </si>
@@ -82,9 +82,6 @@
     <t>CLOSE</t>
   </si>
   <si>
-    <t>Made by: RENEGADEWARE</t>
-  </si>
-  <si>
     <t>season_winter</t>
   </si>
   <si>
@@ -574,12 +571,6 @@
     <t>overworld_1_humid_1</t>
   </si>
   <si>
-    <t>Notice how humidity tends to be higher in large forest and jungle areas, such as the Amazon rainforest.</t>
-  </si>
-  <si>
-    <t>Now go ahead and find a place for the frogs to land. Simply click around the map to find the spot.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remember to make use of the temperature and humidity reading. </t>
   </si>
   <si>
@@ -601,9 +592,6 @@
     <t>overworld_1_analyze_2</t>
   </si>
   <si>
-    <t>Since the earth rotate at a slightly tilted axis around the sun, the atmosphere can change throughout the year.</t>
-  </si>
-  <si>
     <t>Why don’t we adjust the time by selecting a different season.</t>
   </si>
   <si>
@@ -619,15 +607,9 @@
     <t>overworld_1_investigate_1</t>
   </si>
   <si>
-    <t>On the lefthand side of the map are the latitude values. This is the angular distance relative to the earth’s equator (middle of the map).</t>
-  </si>
-  <si>
     <t>Hint: we are looking for a temperate climate, perhaps somewhere in North America...</t>
   </si>
   <si>
-    <t>Looks like the temperature is too low. We will need to change the time of the year to land on this spot.</t>
-  </si>
-  <si>
     <t>colony_1_intro_0</t>
   </si>
   <si>
@@ -829,9 +811,6 @@
     <t>overworld_2_post_intro_2</t>
   </si>
   <si>
-    <t>Anyhow, let’s find places where the wind might by strong. Try looking for areas prone to hurricanes along coastal regions.</t>
-  </si>
-  <si>
     <t>Remember to check the different seasons to see how the wind changes to various positions across Earth.</t>
   </si>
   <si>
@@ -1051,9 +1030,6 @@
     <t>Since we can’t place plants on these rigid grounds, we’ll once again need the help of landscapers to shape the land.</t>
   </si>
   <si>
-    <t>You won’t have to worry about where to place the water thank this time around.</t>
-  </si>
-  <si>
     <t>We will be able to proceed once the frog population has increased.</t>
   </si>
   <si>
@@ -1105,7 +1081,37 @@
     <t>They are expressing their gratitude, and are ready to cooperate.</t>
   </si>
   <si>
-    <t>Well, we can’t just let them hang about in outer space. Besides, it’s not often we are visited by sentient beings, and frogs at that!</t>
+    <t>RENEGADEWARE 2023</t>
+  </si>
+  <si>
+    <t>Since the earth rotates at a slightly tilted axis around the sun, the atmosphere can change throughout the year.</t>
+  </si>
+  <si>
+    <t>Looks like the temperature is too low. We will need to change when to land on this spot.</t>
+  </si>
+  <si>
+    <t>Well, we can’t just let them hang about in outer space. Besides, it’s not often we are visited by sentient beings, and frogs no less!</t>
+  </si>
+  <si>
+    <t>On the lefthand side of the map are the latitude values. This is the angular distance relative to the earth’s equator.</t>
+  </si>
+  <si>
+    <t>overworld_1_temp_1</t>
+  </si>
+  <si>
+    <t>This is due to the earth's equator facing more directly towards the sun.</t>
+  </si>
+  <si>
+    <t>Notice how humidity tends to be higher in areas with large amounts of trees, such as the Amazon rainforest.</t>
+  </si>
+  <si>
+    <t>Now go ahead and find a place for the frogs to land. Simply press on the map to find the spot.</t>
+  </si>
+  <si>
+    <t>Anyhow, let’s find places where the wind might be strong. Try looking for areas prone to hurricanes along coastal regions.</t>
+  </si>
+  <si>
+    <t>You won’t have to worry about where to place the water tank this time around.</t>
   </si>
 </sst>
 </file>
@@ -1444,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D180"/>
+  <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,7 +1483,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1485,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1546,1371 +1552,1379 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>104</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>108</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>110</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B78" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B80" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>161</v>
+      </c>
+      <c r="B83" t="s">
         <v>162</v>
-      </c>
-      <c r="B83" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" t="s">
         <v>166</v>
-      </c>
-      <c r="B84" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" t="s">
         <v>168</v>
-      </c>
-      <c r="B85" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" t="s">
         <v>172</v>
-      </c>
-      <c r="B87" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" t="s">
         <v>174</v>
-      </c>
-      <c r="B88" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B89" t="s">
-        <v>199</v>
+        <v>357</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B90" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>178</v>
+      </c>
+      <c r="B91" t="s">
         <v>179</v>
-      </c>
-      <c r="B91" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>358</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>359</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B94" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B95" t="s">
-        <v>186</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B96" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B97" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B98" t="s">
-        <v>193</v>
+        <v>355</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B99" t="s">
-        <v>194</v>
+        <v>354</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B100" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B101" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B102" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>206</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
+      </c>
+      <c r="B104" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>208</v>
-      </c>
-      <c r="B105" t="s">
-        <v>211</v>
+        <v>200</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B106" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B107" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B108" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B109" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>217</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
+      </c>
+      <c r="B110" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>220</v>
-      </c>
-      <c r="B111" t="s">
-        <v>224</v>
+        <v>211</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B112" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>226</v>
+        <v>215</v>
+      </c>
+      <c r="B113" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>223</v>
-      </c>
-      <c r="B114" t="s">
-        <v>250</v>
+        <v>216</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B115" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B116" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B117" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B118" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B119" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B120" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>234</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>236</v>
+        <v>227</v>
+      </c>
+      <c r="B121" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>238</v>
-      </c>
-      <c r="B123" t="s">
-        <v>241</v>
+        <v>229</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>239</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>242</v>
+        <v>232</v>
+      </c>
+      <c r="B124" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>240</v>
-      </c>
-      <c r="B125" t="s">
-        <v>256</v>
+        <v>233</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B126" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B127" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B128" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B129" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B130" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B131" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B132" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>262</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>273</v>
+        <v>255</v>
+      </c>
+      <c r="B133" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>263</v>
-      </c>
-      <c r="B134" t="s">
-        <v>274</v>
+        <v>256</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>264</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>265</v>
+        <v>257</v>
+      </c>
+      <c r="B135" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>266</v>
-      </c>
-      <c r="B136" t="s">
-        <v>269</v>
+        <v>258</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>267</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>270</v>
+        <v>260</v>
+      </c>
+      <c r="B137" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>359</v>
+        <v>263</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>275</v>
-      </c>
-      <c r="B139" t="s">
-        <v>278</v>
+        <v>262</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B140" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B141" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="B142" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B143" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B144" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="B145" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>288</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>291</v>
+        <v>280</v>
+      </c>
+      <c r="B146" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>289</v>
-      </c>
-      <c r="B147" t="s">
-        <v>292</v>
+        <v>281</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="B148" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B149" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B150" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B151" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>297</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>302</v>
+        <v>289</v>
+      </c>
+      <c r="B152" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>304</v>
-      </c>
-      <c r="B154" t="s">
-        <v>306</v>
+        <v>296</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="B155" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B156" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B157" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>313</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>315</v>
+        <v>302</v>
+      </c>
+      <c r="B158" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>314</v>
-      </c>
-      <c r="B159" t="s">
-        <v>316</v>
+        <v>306</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="B160" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>318</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>320</v>
+        <v>310</v>
+      </c>
+      <c r="B161" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>335</v>
-      </c>
-      <c r="B169" t="s">
-        <v>337</v>
+        <v>325</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B170" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="B171" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>340</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>343</v>
+        <v>332</v>
+      </c>
+      <c r="B172" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>344</v>
+        <v>363</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>356</v>
-      </c>
-      <c r="B177" t="s">
-        <v>358</v>
-      </c>
-      <c r="C177">
-        <v>3</v>
+        <v>339</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B178" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C178">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>352</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>353</v>
+        <v>343</v>
+      </c>
+      <c r="B179" t="s">
+        <v>349</v>
       </c>
       <c r="C179">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>355</v>
+        <v>345</v>
+      </c>
+      <c r="C180">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>346</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more overworld hotspot refactor
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C9C9C8-33B5-4938-A981-47C1B532E38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC592A0-E42F-4D43-B3C2-80A0AB4FFB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5310" yWindow="2550" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="368">
   <si>
     <t>Key</t>
   </si>
@@ -1112,6 +1112,18 @@
   </si>
   <si>
     <t>You won’t have to worry about where to place the water tank this time around.</t>
+  </si>
+  <si>
+    <t>analyze</t>
+  </si>
+  <si>
+    <t>ANALYZE</t>
+  </si>
+  <si>
+    <t>analyzeWait</t>
+  </si>
+  <si>
+    <t>AWAITING ANALYSIS</t>
   </si>
 </sst>
 </file>
@@ -1450,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D181"/>
+  <dimension ref="A1:D183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+      <selection activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2927,6 +2939,22 @@
         <v>347</v>
       </c>
     </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>364</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>366</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
adjusted hotspot analyze overlay to prevent overlap with hud on some overworld levels, over. Fixed some bugs with hotspot selecting.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC592A0-E42F-4D43-B3C2-80A0AB4FFB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2161922-9A2E-40DC-8100-1E2192346537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5310" yWindow="2550" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1464,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,1355 +1604,1355 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>364</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>366</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>164</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>21</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>43</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>149</v>
-      </c>
-      <c r="B75" t="s">
-        <v>147</v>
+        <v>108</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>150</v>
-      </c>
-      <c r="B76" t="s">
-        <v>157</v>
+        <v>110</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B78" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>153</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>356</v>
+        <v>151</v>
+      </c>
+      <c r="B79" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>352</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>159</v>
+        <v>356</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>156</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
+      </c>
+      <c r="B82" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>161</v>
-      </c>
-      <c r="B83" t="s">
-        <v>162</v>
+        <v>155</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>165</v>
-      </c>
-      <c r="B84" t="s">
-        <v>166</v>
+        <v>156</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>169</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
+      </c>
+      <c r="B86" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>173</v>
-      </c>
-      <c r="B88" t="s">
-        <v>174</v>
+        <v>169</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B89" t="s">
-        <v>357</v>
+        <v>172</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>179</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>358</v>
+        <v>177</v>
       </c>
       <c r="B92" t="s">
-        <v>359</v>
+        <v>176</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B93" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>182</v>
+        <v>358</v>
       </c>
       <c r="B94" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s">
-        <v>361</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B96" t="s">
-        <v>183</v>
+        <v>360</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B97" t="s">
-        <v>195</v>
+        <v>361</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B98" t="s">
-        <v>355</v>
+        <v>183</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B99" t="s">
-        <v>354</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B100" t="s">
-        <v>190</v>
+        <v>355</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B101" t="s">
-        <v>192</v>
+        <v>354</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B102" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B103" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>200</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
+      </c>
+      <c r="B105" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B106" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>203</v>
-      </c>
-      <c r="B107" t="s">
-        <v>206</v>
+        <v>200</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B108" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B109" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B110" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>211</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+      <c r="B111" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B112" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>215</v>
-      </c>
-      <c r="B113" t="s">
-        <v>219</v>
+        <v>211</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>216</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
+      </c>
+      <c r="B114" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B115" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>221</v>
-      </c>
-      <c r="B116" t="s">
-        <v>245</v>
+        <v>216</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B117" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B118" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B119" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B120" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B121" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>228</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
+      </c>
+      <c r="B122" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>229</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
+      </c>
+      <c r="B123" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>232</v>
-      </c>
-      <c r="B124" t="s">
-        <v>235</v>
+        <v>228</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B126" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>237</v>
-      </c>
-      <c r="B127" t="s">
-        <v>251</v>
+        <v>233</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B128" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B129" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B130" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B131" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="B132" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B133" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>256</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>266</v>
+        <v>253</v>
+      </c>
+      <c r="B134" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B135" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B137" t="s">
-        <v>362</v>
+        <v>267</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>262</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>351</v>
+        <v>260</v>
+      </c>
+      <c r="B139" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>268</v>
-      </c>
-      <c r="B140" t="s">
-        <v>271</v>
+        <v>261</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>269</v>
-      </c>
-      <c r="B141" t="s">
-        <v>272</v>
+        <v>262</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B142" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B143" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B144" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B145" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B146" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>281</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>284</v>
+        <v>276</v>
+      </c>
+      <c r="B147" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B148" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>286</v>
-      </c>
-      <c r="B149" t="s">
-        <v>291</v>
+        <v>281</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B150" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B151" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B152" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>290</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>295</v>
+        <v>288</v>
+      </c>
+      <c r="B153" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>296</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>298</v>
+        <v>289</v>
+      </c>
+      <c r="B154" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>297</v>
-      </c>
-      <c r="B155" t="s">
-        <v>299</v>
+        <v>290</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>300</v>
-      </c>
-      <c r="B156" t="s">
-        <v>303</v>
+        <v>296</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B157" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B158" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>306</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>308</v>
+        <v>301</v>
+      </c>
+      <c r="B159" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B160" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>310</v>
-      </c>
-      <c r="B161" t="s">
-        <v>312</v>
+        <v>306</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>311</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
+      </c>
+      <c r="B162" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>314</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>315</v>
+        <v>310</v>
+      </c>
+      <c r="B163" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>328</v>
-      </c>
-      <c r="B170" t="s">
-        <v>330</v>
+        <v>324</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>329</v>
-      </c>
-      <c r="B171" t="s">
-        <v>331</v>
+        <v>325</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B172" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>333</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>363</v>
+        <v>329</v>
+      </c>
+      <c r="B173" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>334</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
+      </c>
+      <c r="B174" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>340</v>
+        <v>363</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>348</v>
-      </c>
-      <c r="B178" t="s">
-        <v>350</v>
-      </c>
-      <c r="C178">
-        <v>3</v>
+        <v>338</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>343</v>
-      </c>
-      <c r="B179" t="s">
-        <v>349</v>
-      </c>
-      <c r="C179">
-        <v>8</v>
+        <v>339</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>344</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>345</v>
+        <v>348</v>
+      </c>
+      <c r="B180" t="s">
+        <v>350</v>
       </c>
       <c r="C180">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>346</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
+      </c>
+      <c r="B181" t="s">
+        <v>349</v>
+      </c>
+      <c r="C181">
+        <v>8</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>365</v>
+        <v>345</v>
+      </c>
+      <c r="C182">
+        <v>5</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tutorial update for overworld01
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2161922-9A2E-40DC-8100-1E2192346537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4C26F2-D162-4061-A45C-832C301F9A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5310" yWindow="2550" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="374">
   <si>
     <t>Key</t>
   </si>
@@ -565,9 +565,6 @@
     <t>overworld_1_humid_0</t>
   </si>
   <si>
-    <t>Next is the humidity readings of Earth. The percentage tells us how much water vapor is present on air.</t>
-  </si>
-  <si>
     <t>overworld_1_humid_1</t>
   </si>
   <si>
@@ -580,9 +577,6 @@
     <t>overworld_1_hotspot_1</t>
   </si>
   <si>
-    <t>overworld_1_hotspot_2</t>
-  </si>
-  <si>
     <t>overworld_1_analyze_0</t>
   </si>
   <si>
@@ -592,9 +586,6 @@
     <t>overworld_1_analyze_2</t>
   </si>
   <si>
-    <t>Why don’t we adjust the time by selecting a different season.</t>
-  </si>
-  <si>
     <t>overworld_1_investigate_0</t>
   </si>
   <si>
@@ -607,9 +598,6 @@
     <t>overworld_1_investigate_1</t>
   </si>
   <si>
-    <t>Hint: we are looking for a temperate climate, perhaps somewhere in North America...</t>
-  </si>
-  <si>
     <t>colony_1_intro_0</t>
   </si>
   <si>
@@ -1102,12 +1090,6 @@
     <t>This is due to the earth's equator facing more directly towards the sun.</t>
   </si>
   <si>
-    <t>Notice how humidity tends to be higher in areas with large amounts of trees, such as the Amazon rainforest.</t>
-  </si>
-  <si>
-    <t>Now go ahead and find a place for the frogs to land. Simply press on the map to find the spot.</t>
-  </si>
-  <si>
     <t>Anyhow, let’s find places where the wind might be strong. Try looking for areas prone to hurricanes along coastal regions.</t>
   </si>
   <si>
@@ -1124,13 +1106,49 @@
   </si>
   <si>
     <t>AWAITING ANALYSIS</t>
+  </si>
+  <si>
+    <t>Notice how humidity tends to be higher near the equator? This coincides with the temperature being high, allowing air to hold more water.</t>
+  </si>
+  <si>
+    <t>overworld_1_humid_2</t>
+  </si>
+  <si>
+    <t>It’s no wonder there is an abundance of trees in these regions!</t>
+  </si>
+  <si>
+    <t>Now go ahead and find a place for the frogs to land. Simply press on the map to find the hotspot.</t>
+  </si>
+  <si>
+    <t>overworld_1_hotspot_found_0</t>
+  </si>
+  <si>
+    <t>overworld_1_hotspot_found_1</t>
+  </si>
+  <si>
+    <t>Why don’t we adjust the time by selecting a different season. Perhaps summer will give us the temperature to satisfy the criteria!</t>
+  </si>
+  <si>
+    <t>Next is the humidity readings of Earth. The percentage tells us the amount of water vapor in the air relative to its capacity based on the current temperature.</t>
+  </si>
+  <si>
+    <t>Now that you have found the hotspot, you’ll need to analyze its temperature and humidity readings.</t>
+  </si>
+  <si>
+    <t>Remember to switch between the temperature and humidity overlay to analyze them both.</t>
+  </si>
+  <si>
+    <t>overworld_1_analyze_3</t>
+  </si>
+  <si>
+    <t>Remember to reanalyze the atmospheric readings when changing seasons.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1142,6 +1160,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1173,7 +1198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1182,6 +1207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1462,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D183"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1529,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,18 +1630,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2127,7 +2153,7 @@
         <v>153</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2135,7 +2161,7 @@
         <v>154</v>
       </c>
       <c r="B82" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2207,7 +2233,7 @@
         <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2228,10 +2254,10 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B94" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2239,720 +2265,744 @@
         <v>180</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>369</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B96" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>363</v>
       </c>
       <c r="B97" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>185</v>
-      </c>
-      <c r="B98" t="s">
         <v>183</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B99" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>187</v>
+        <v>366</v>
       </c>
       <c r="B100" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>188</v>
+        <v>367</v>
       </c>
       <c r="B101" t="s">
-        <v>354</v>
+        <v>371</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B102" t="s">
-        <v>190</v>
+        <v>351</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B103" t="s">
-        <v>192</v>
+        <v>350</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>194</v>
-      </c>
-      <c r="B104" t="s">
-        <v>193</v>
+        <v>187</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>196</v>
-      </c>
-      <c r="B105" t="s">
-        <v>198</v>
+        <v>372</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B106" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>200</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>201</v>
+        <v>191</v>
+      </c>
+      <c r="B107" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B108" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B109" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>204</v>
-      </c>
-      <c r="B110" t="s">
-        <v>207</v>
+        <v>196</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B111" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B112" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>211</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>213</v>
+        <v>200</v>
+      </c>
+      <c r="B113" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B114" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B115" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B117" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B118" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>222</v>
-      </c>
-      <c r="B119" t="s">
-        <v>246</v>
+        <v>212</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B120" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B121" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B122" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B123" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>228</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>230</v>
+        <v>220</v>
+      </c>
+      <c r="B124" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>229</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>231</v>
+        <v>221</v>
+      </c>
+      <c r="B125" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B126" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>234</v>
-      </c>
-      <c r="B128" t="s">
-        <v>250</v>
+        <v>225</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B129" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>238</v>
-      </c>
-      <c r="B130" t="s">
-        <v>241</v>
+        <v>229</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B131" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B132" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="B133" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="B134" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="B135" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>256</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>266</v>
+        <v>248</v>
+      </c>
+      <c r="B136" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B137" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>258</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>259</v>
+        <v>251</v>
+      </c>
+      <c r="B138" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>260</v>
-      </c>
-      <c r="B139" t="s">
-        <v>362</v>
+        <v>252</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>261</v>
-      </c>
-      <c r="B140" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B140" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>351</v>
+        <v>255</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B142" t="s">
-        <v>271</v>
+        <v>356</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>269</v>
-      </c>
-      <c r="B143" t="s">
-        <v>272</v>
+        <v>257</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>270</v>
-      </c>
-      <c r="B144" t="s">
-        <v>273</v>
+        <v>258</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="B145" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B146" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B147" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B148" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>281</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>284</v>
+        <v>271</v>
+      </c>
+      <c r="B149" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B150" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B151" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>287</v>
-      </c>
-      <c r="B152" t="s">
-        <v>292</v>
+        <v>277</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="B153" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B154" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>290</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>295</v>
+        <v>283</v>
+      </c>
+      <c r="B155" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>296</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>298</v>
+        <v>284</v>
+      </c>
+      <c r="B156" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="B157" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>300</v>
-      </c>
-      <c r="B158" t="s">
-        <v>303</v>
+        <v>286</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>301</v>
-      </c>
-      <c r="B159" t="s">
-        <v>304</v>
+        <v>292</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B160" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>306</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>308</v>
+        <v>296</v>
+      </c>
+      <c r="B161" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="B162" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B163" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>314</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>315</v>
+        <v>303</v>
+      </c>
+      <c r="B165" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>316</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>318</v>
+        <v>306</v>
+      </c>
+      <c r="B166" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>328</v>
-      </c>
-      <c r="B172" t="s">
-        <v>330</v>
+        <v>317</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>329</v>
-      </c>
-      <c r="B173" t="s">
-        <v>331</v>
+        <v>320</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>332</v>
-      </c>
-      <c r="B174" t="s">
-        <v>335</v>
+        <v>321</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>333</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>363</v>
+        <v>324</v>
+      </c>
+      <c r="B175" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>334</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>336</v>
+        <v>325</v>
+      </c>
+      <c r="B176" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>337</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>340</v>
+        <v>328</v>
+      </c>
+      <c r="B177" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>341</v>
+        <v>357</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>348</v>
-      </c>
-      <c r="B180" t="s">
-        <v>350</v>
-      </c>
-      <c r="C180">
-        <v>3</v>
+        <v>333</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>343</v>
-      </c>
-      <c r="B181" t="s">
-        <v>349</v>
-      </c>
-      <c r="C181">
-        <v>8</v>
+        <v>334</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="C182">
-        <v>5</v>
+        <v>338</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>344</v>
+      </c>
+      <c r="B183" t="s">
         <v>346</v>
       </c>
-      <c r="B183" s="3" t="s">
-        <v>347</v>
+      <c r="C183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>339</v>
+      </c>
+      <c r="B184" t="s">
+        <v>345</v>
+      </c>
+      <c r="C184">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>340</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C185">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>342</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revamped tutorial and lessons in overworld02 (Coriolis effect and ocean current stuff)
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4C26F2-D162-4061-A45C-832C301F9A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEC637B-5232-4ED0-95B7-3AFD30FD02E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="2550" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39375" yWindow="1335" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="390">
   <si>
     <t>Key</t>
   </si>
@@ -778,18 +778,6 @@
     <t>overworld_2_wind_0</t>
   </si>
   <si>
-    <t>overworld_2_wind_temp_0</t>
-  </si>
-  <si>
-    <t>overworld_2_wind_temp_1</t>
-  </si>
-  <si>
-    <t>overworld_2_wind_temp_2</t>
-  </si>
-  <si>
-    <t>This cycle continues as the wind travels, building up more speed along the way.</t>
-  </si>
-  <si>
     <t>overworld_2_post_intro_0</t>
   </si>
   <si>
@@ -805,15 +793,6 @@
     <t>Our next batch of frogs are keen on living in a windy environment, as well as hot and humid.</t>
   </si>
   <si>
-    <t>Notice the winds forming into a swirly motion? These are tropical cyclones, sometimes referred to as: hurricanes, or typhoons.</t>
-  </si>
-  <si>
-    <t>As you can see, the warm energy from the ocean rises, forming low pressure from below. This causes more air to fill in.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The air filling in must then rise because of the heat, accumulating water which release more heat. </t>
-  </si>
-  <si>
     <t>colony_2_intro_0</t>
   </si>
   <si>
@@ -1142,6 +1121,75 @@
   </si>
   <si>
     <t>Remember to reanalyze the atmospheric readings when changing seasons.</t>
+  </si>
+  <si>
+    <t>lowPressure</t>
+  </si>
+  <si>
+    <t>Low Pressure</t>
+  </si>
+  <si>
+    <t>highPressure</t>
+  </si>
+  <si>
+    <t>High Pressure</t>
+  </si>
+  <si>
+    <t>overworld_2_wind_1</t>
+  </si>
+  <si>
+    <t>overworld_2_wind_2</t>
+  </si>
+  <si>
+    <t>Notice how the winds tend to travel diagonally across Earth? This is due to the Coriolis effect.</t>
+  </si>
+  <si>
+    <t>Let’s take a look again on the map.</t>
+  </si>
+  <si>
+    <t>overworld_2_coriolis_0</t>
+  </si>
+  <si>
+    <t>overworld_2_coriolis_1</t>
+  </si>
+  <si>
+    <t>overworld_2_coriolis_2</t>
+  </si>
+  <si>
+    <t>overworld_2_wind_3</t>
+  </si>
+  <si>
+    <t>These are the general directions of the global winds. As warm air from the equator rises up, it cools down and sinks towards north or south.</t>
+  </si>
+  <si>
+    <t>Sometimes, interactions between the low- and high-pressure winds will cause a cyclone, such as the ones you see on the map.</t>
+  </si>
+  <si>
+    <t>This is called a hurricane in the Atlantic Ocean, and a typhoon in the Pacific Ocean.</t>
+  </si>
+  <si>
+    <t>overworld_2_ocean_0</t>
+  </si>
+  <si>
+    <t>One other thing to note is how the wind drives the surface ocean currents, which help regulates the temperature across the lands.</t>
+  </si>
+  <si>
+    <t>overworld_2_gulf_stream_0</t>
+  </si>
+  <si>
+    <t>overworld_2_gulf_stream_1</t>
+  </si>
+  <si>
+    <t>Here is an example of an ocean current that brings warm water from the equator towards north, known as the Gulf Stream.</t>
+  </si>
+  <si>
+    <t>The Gulf Stream’s warm waters maintain a relatively warm temperature in the nearby lands throughout the year.</t>
+  </si>
+  <si>
+    <t>Since Earth spins from west to east, the winds in the northern hemisphere blow northwest to southeast, and vice-versa in the southern hemisphere.</t>
+  </si>
+  <si>
+    <t>These cyclones can become dangerous as it accumulates wind speed and heavy amounts of water, as it travels across the land.</t>
   </si>
 </sst>
 </file>
@@ -1488,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D186"/>
+  <dimension ref="A1:D194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1577,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,18 +1678,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1726,1283 +1774,1347 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>367</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>51</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>369</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>21</v>
+        <v>370</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>43</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>39</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>149</v>
-      </c>
-      <c r="B77" t="s">
-        <v>147</v>
+        <v>108</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>150</v>
-      </c>
-      <c r="B78" t="s">
-        <v>157</v>
+        <v>110</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>153</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>352</v>
+        <v>151</v>
+      </c>
+      <c r="B81" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B82" t="s">
-        <v>348</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>159</v>
+        <v>345</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>156</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
+      </c>
+      <c r="B84" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>161</v>
-      </c>
-      <c r="B85" t="s">
-        <v>162</v>
+        <v>155</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>165</v>
-      </c>
-      <c r="B86" t="s">
-        <v>166</v>
+        <v>156</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B87" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>169</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
+      </c>
+      <c r="B88" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B89" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>173</v>
-      </c>
-      <c r="B90" t="s">
-        <v>174</v>
+        <v>169</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>353</v>
+        <v>172</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B92" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B93" t="s">
-        <v>179</v>
+        <v>346</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>354</v>
+        <v>177</v>
       </c>
       <c r="B94" t="s">
-        <v>355</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B95" t="s">
-        <v>369</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>181</v>
+        <v>347</v>
       </c>
       <c r="B96" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>363</v>
+        <v>180</v>
       </c>
       <c r="B97" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>183</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>365</v>
+        <v>181</v>
+      </c>
+      <c r="B98" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>184</v>
+        <v>356</v>
       </c>
       <c r="B99" t="s">
-        <v>182</v>
+        <v>357</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>366</v>
-      </c>
-      <c r="B100" t="s">
-        <v>370</v>
+        <v>183</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>367</v>
+        <v>184</v>
       </c>
       <c r="B101" t="s">
-        <v>371</v>
+        <v>182</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>185</v>
+        <v>359</v>
       </c>
       <c r="B102" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>186</v>
+        <v>360</v>
       </c>
       <c r="B103" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>187</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>368</v>
+        <v>185</v>
+      </c>
+      <c r="B104" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>372</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>373</v>
+        <v>186</v>
+      </c>
+      <c r="B105" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>188</v>
-      </c>
-      <c r="B106" t="s">
-        <v>189</v>
+        <v>187</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>191</v>
-      </c>
-      <c r="B107" t="s">
-        <v>190</v>
+        <v>365</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B108" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B109" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>196</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
+      </c>
+      <c r="B110" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B111" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>199</v>
-      </c>
-      <c r="B112" t="s">
-        <v>202</v>
+        <v>196</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B113" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B114" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B115" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>207</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+      <c r="B116" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B117" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>211</v>
-      </c>
-      <c r="B118" t="s">
-        <v>215</v>
+        <v>207</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>212</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
+      </c>
+      <c r="B119" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B120" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>217</v>
-      </c>
-      <c r="B121" t="s">
-        <v>241</v>
+        <v>212</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B122" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B123" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B124" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B125" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B126" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>224</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
+      </c>
+      <c r="B127" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>225</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
+      </c>
+      <c r="B128" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>228</v>
-      </c>
-      <c r="B129" t="s">
-        <v>231</v>
+        <v>224</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B131" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>233</v>
-      </c>
-      <c r="B132" t="s">
-        <v>247</v>
+        <v>229</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B133" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B134" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B135" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="B136" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="B137" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B138" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>252</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
+      </c>
+      <c r="B139" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>253</v>
+        <v>375</v>
       </c>
       <c r="B140" t="s">
-        <v>263</v>
+        <v>373</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>254</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>255</v>
+        <v>376</v>
+      </c>
+      <c r="B141" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>256</v>
-      </c>
-      <c r="B142" t="s">
-        <v>356</v>
+        <v>377</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>257</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>259</v>
+        <v>251</v>
+      </c>
+      <c r="B143" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>258</v>
+        <v>371</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>264</v>
+        <v>372</v>
       </c>
       <c r="B145" t="s">
-        <v>267</v>
+        <v>389</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>265</v>
-      </c>
-      <c r="B146" t="s">
-        <v>268</v>
+        <v>378</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>266</v>
-      </c>
-      <c r="B147" t="s">
-        <v>269</v>
+        <v>382</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>270</v>
-      </c>
-      <c r="B148" t="s">
-        <v>273</v>
+        <v>384</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>271</v>
-      </c>
-      <c r="B149" t="s">
-        <v>274</v>
+        <v>385</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="B150" t="s">
-        <v>275</v>
+        <v>349</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>276</v>
-      </c>
-      <c r="B151" t="s">
-        <v>279</v>
+        <v>253</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>280</v>
+        <v>340</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="B153" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="B154" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="B155" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="B156" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="B157" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>286</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>291</v>
+        <v>265</v>
+      </c>
+      <c r="B158" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>292</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>294</v>
+        <v>269</v>
+      </c>
+      <c r="B159" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>293</v>
-      </c>
-      <c r="B160" t="s">
-        <v>295</v>
+        <v>270</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="B161" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="B162" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="B163" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>302</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>304</v>
+        <v>277</v>
+      </c>
+      <c r="B164" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="B165" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>306</v>
-      </c>
-      <c r="B166" t="s">
-        <v>308</v>
+        <v>279</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>310</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>311</v>
+        <v>286</v>
+      </c>
+      <c r="B168" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>312</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>314</v>
+        <v>289</v>
+      </c>
+      <c r="B169" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>313</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>315</v>
+        <v>290</v>
+      </c>
+      <c r="B170" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>316</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>318</v>
+        <v>291</v>
+      </c>
+      <c r="B171" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>320</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>322</v>
+        <v>296</v>
+      </c>
+      <c r="B173" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>321</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>323</v>
+        <v>299</v>
+      </c>
+      <c r="B174" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>324</v>
-      </c>
-      <c r="B175" t="s">
-        <v>326</v>
+        <v>300</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>325</v>
-      </c>
-      <c r="B176" t="s">
-        <v>327</v>
+        <v>303</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>328</v>
-      </c>
-      <c r="B177" t="s">
-        <v>331</v>
+        <v>305</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>357</v>
+        <v>308</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="B183" t="s">
-        <v>346</v>
-      </c>
-      <c r="C183">
-        <v>3</v>
+        <v>319</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="B184" t="s">
-        <v>345</v>
-      </c>
-      <c r="C184">
-        <v>8</v>
+        <v>320</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>340</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="C185">
-        <v>5</v>
+        <v>321</v>
+      </c>
+      <c r="B185" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>343</v>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>323</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>326</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>327</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>328</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>337</v>
+      </c>
+      <c r="B191" t="s">
+        <v>339</v>
+      </c>
+      <c r="C191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>332</v>
+      </c>
+      <c r="B192" t="s">
+        <v>338</v>
+      </c>
+      <c r="C192">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>333</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C193">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>335</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaked levels to be shorter, some stats tweak to make the game a little less rough. some language tweaks. new build for submit.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEC637B-5232-4ED0-95B7-3AFD30FD02E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B2D07B-0F39-4C10-9091-B17B6F847A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39375" yWindow="1335" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8070" yWindow="2595" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -1069,9 +1069,6 @@
     <t>This is due to the earth's equator facing more directly towards the sun.</t>
   </si>
   <si>
-    <t>Anyhow, let’s find places where the wind might be strong. Try looking for areas prone to hurricanes along coastal regions.</t>
-  </si>
-  <si>
     <t>You won’t have to worry about where to place the water tank this time around.</t>
   </si>
   <si>
@@ -1165,9 +1162,6 @@
     <t>Sometimes, interactions between the low- and high-pressure winds will cause a cyclone, such as the ones you see on the map.</t>
   </si>
   <si>
-    <t>This is called a hurricane in the Atlantic Ocean, and a typhoon in the Pacific Ocean.</t>
-  </si>
-  <si>
     <t>overworld_2_ocean_0</t>
   </si>
   <si>
@@ -1190,6 +1184,12 @@
   </si>
   <si>
     <t>These cyclones can become dangerous as it accumulates wind speed and heavy amounts of water, as it travels across the land.</t>
+  </si>
+  <si>
+    <t>Anyhow, let’s find places where the wind might be strong. Try looking for areas prone to hurricanes, or typhoons along coastal regions.</t>
+  </si>
+  <si>
+    <t>These are often called hurricanes in the Atlantic Ocean, and typhoons in the Pacific Ocean.</t>
   </si>
 </sst>
 </file>
@@ -1539,7 +1539,7 @@
   <dimension ref="A1:D194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,18 +1678,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>350</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>352</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1774,18 +1774,18 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>366</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>368</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2329,7 +2329,7 @@
         <v>180</v>
       </c>
       <c r="B97" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2337,15 +2337,15 @@
         <v>181</v>
       </c>
       <c r="B98" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>355</v>
+      </c>
+      <c r="B99" t="s">
         <v>356</v>
-      </c>
-      <c r="B99" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2353,7 +2353,7 @@
         <v>183</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2366,18 +2366,18 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B103" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2401,15 +2401,15 @@
         <v>187</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>364</v>
+      </c>
+      <c r="B107" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2670,26 +2670,26 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B140" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B141" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -2697,55 +2697,55 @@
         <v>251</v>
       </c>
       <c r="B143" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B145" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>378</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>382</v>
+      </c>
+      <c r="B148" s="3" t="s">
         <v>384</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>383</v>
+      </c>
+      <c r="B149" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -2753,7 +2753,7 @@
         <v>252</v>
       </c>
       <c r="B150" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -3041,7 +3041,7 @@
         <v>322</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added latitude illustration, added dialog display at top, highlight to atmosphere and season toggle when it becomes available.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B2D07B-0F39-4C10-9091-B17B6F847A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A19B825-2532-49B1-BDCC-4E29C1C6D433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="2595" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="195" yWindow="2775" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -496,9 +496,6 @@
     <t>They appear to be frog-like. Let me put on my frog suit to communicate with these peculiar creatures!</t>
   </si>
   <si>
-    <t>It looks like they have been exiled from their planet, and are looking for a new home.</t>
-  </si>
-  <si>
     <t>Well, why not? Let’s give these hapless frogs some proper homes to settle in. There’s still plenty of room here on Earth.</t>
   </si>
   <si>
@@ -547,15 +544,9 @@
     <t>In this case, we need to find a place where it’s fairly warm and humid.</t>
   </si>
   <si>
-    <t>overworld_1_hud_0</t>
-  </si>
-  <si>
     <t>Now let’s view the temperature readings of Earth.</t>
   </si>
   <si>
-    <t>overworld_1_hud_1</t>
-  </si>
-  <si>
     <t>overworld_1_temp_0</t>
   </si>
   <si>
@@ -718,9 +709,6 @@
     <t>Watch out! It looks like weeds are starting to grow on one of the structures!</t>
   </si>
   <si>
-    <t>Though the weather is ideal for the frogs, unfortunately so it will be for these invasive plants.</t>
-  </si>
-  <si>
     <t>colony_1_mole_0</t>
   </si>
   <si>
@@ -802,9 +790,6 @@
     <t>colony_2_intro_2</t>
   </si>
   <si>
-    <t>Looks like we’ve landed in a tropical climate. Where it’s hot and humid all year round with plenty of rain.</t>
-  </si>
-  <si>
     <t>Though it looks like we’re getting more rain than usual, something is afoot...</t>
   </si>
   <si>
@@ -838,15 +823,9 @@
     <t>colony_2_fly_2</t>
   </si>
   <si>
-    <t>Look out, it's a beetle!</t>
-  </si>
-  <si>
     <t>Due to the consistent warmth in tropical climates, insects are able to thrive throughout the year.</t>
   </si>
   <si>
-    <t>These troublesome insects can be dealt with by a hero frog. Make sure to have one around to rout them out.</t>
-  </si>
-  <si>
     <t>colony_2_hazzard_0</t>
   </si>
   <si>
@@ -862,9 +841,6 @@
     <t>colony_2_hazzard_4</t>
   </si>
   <si>
-    <t>Take cover, a hurricane is heading our way!</t>
-  </si>
-  <si>
     <t>As mentioned before about hurricanes: the wind speed that has accumulated over low pressure from the surface has reached critical speed.</t>
   </si>
   <si>
@@ -1042,18 +1018,9 @@
     <t>CONGRATULATIONS</t>
   </si>
   <si>
-    <t>This time around, there are more than one hotspot to discover on the map. Only one of them will match with the frogs’ criteria.</t>
-  </si>
-  <si>
-    <t>They are expressing their gratitude, and are ready to cooperate.</t>
-  </si>
-  <si>
     <t>RENEGADEWARE 2023</t>
   </si>
   <si>
-    <t>Since the earth rotates at a slightly tilted axis around the sun, the atmosphere can change throughout the year.</t>
-  </si>
-  <si>
     <t>Looks like the temperature is too low. We will need to change when to land on this spot.</t>
   </si>
   <si>
@@ -1102,9 +1069,6 @@
     <t>overworld_1_hotspot_found_1</t>
   </si>
   <si>
-    <t>Why don’t we adjust the time by selecting a different season. Perhaps summer will give us the temperature to satisfy the criteria!</t>
-  </si>
-  <si>
     <t>Next is the humidity readings of Earth. The percentage tells us the amount of water vapor in the air relative to its capacity based on the current temperature.</t>
   </si>
   <si>
@@ -1190,6 +1154,42 @@
   </si>
   <si>
     <t>These are often called hurricanes in the Atlantic Ocean, and typhoons in the Pacific Ocean.</t>
+  </si>
+  <si>
+    <t>It looks like they have been exiled from their planet and are looking for a new home.</t>
+  </si>
+  <si>
+    <t>They are expressing their gratitude and are ready to cooperate.</t>
+  </si>
+  <si>
+    <t>Since the earth rotates at a slightly tilted axis around the Sun, the atmosphere can change throughout the year.</t>
+  </si>
+  <si>
+    <t>Let's adjust the time by selecting a different season. Perhaps summer will give us the temperature to satisfy the criteria!</t>
+  </si>
+  <si>
+    <t>Though the weather is ideal for the frogs, unfortunately, it is also ideal for these invasive plants.</t>
+  </si>
+  <si>
+    <t>This time around, there is more than one hotspot to discover on the map. Only one of them will match with the frogs’ criteria.</t>
+  </si>
+  <si>
+    <t>Looks like we’ve landed in a tropical climate, where it’s hot and humid all year round with plenty of rain.</t>
+  </si>
+  <si>
+    <t>Look out! It's a beetle!</t>
+  </si>
+  <si>
+    <t>These troublesome insects can be dealt with by a hero frog. Make sure to have one around to get them out.</t>
+  </si>
+  <si>
+    <t>Take cover! A hurricane is heading our way!</t>
+  </si>
+  <si>
+    <t>overworld_1_latitude_0</t>
+  </si>
+  <si>
+    <t>overworld_1_temp_intro_0</t>
   </si>
 </sst>
 </file>
@@ -1538,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1577,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1678,18 +1678,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1766,26 +1766,26 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2209,7 +2209,7 @@
         <v>152</v>
       </c>
       <c r="B82" t="s">
-        <v>158</v>
+        <v>378</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
         <v>153</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2225,7 +2225,7 @@
         <v>154</v>
       </c>
       <c r="B84" t="s">
-        <v>341</v>
+        <v>379</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
         <v>155</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2241,847 +2241,847 @@
         <v>156</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" t="s">
         <v>161</v>
-      </c>
-      <c r="B87" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" t="s">
         <v>165</v>
-      </c>
-      <c r="B88" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" t="s">
         <v>167</v>
-      </c>
-      <c r="B89" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>170</v>
+      </c>
+      <c r="B91" t="s">
         <v>171</v>
-      </c>
-      <c r="B91" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>172</v>
+      </c>
+      <c r="B92" t="s">
         <v>173</v>
-      </c>
-      <c r="B92" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>175</v>
+        <v>388</v>
       </c>
       <c r="B93" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>177</v>
+        <v>389</v>
       </c>
       <c r="B94" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B95" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="B96" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B97" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B98" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="B99" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B101" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="B102" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="B103" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B104" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
-        <v>343</v>
+        <v>380</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B108" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B109" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B110" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>195</v>
+      </c>
+      <c r="B113" t="s">
         <v>198</v>
-      </c>
-      <c r="B113" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>196</v>
+      </c>
+      <c r="B114" t="s">
         <v>199</v>
-      </c>
-      <c r="B114" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>197</v>
+      </c>
+      <c r="B115" t="s">
         <v>200</v>
-      </c>
-      <c r="B115" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B116" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>202</v>
+      </c>
+      <c r="B117" t="s">
         <v>205</v>
-      </c>
-      <c r="B117" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B119" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B120" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B122" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B123" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B124" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B125" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B126" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B127" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B128" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>225</v>
+      </c>
+      <c r="B131" t="s">
         <v>228</v>
-      </c>
-      <c r="B131" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>232</v>
+        <v>382</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B133" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B134" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B135" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B136" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B137" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B138" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B139" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="B140" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="B141" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B143" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="B145" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>365</v>
+      </c>
+      <c r="B146" s="4" t="s">
         <v>377</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B150" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>340</v>
+        <v>383</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B153" t="s">
-        <v>260</v>
+        <v>384</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B154" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B155" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B156" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B157" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B158" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B159" t="s">
-        <v>272</v>
+        <v>385</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B161" t="s">
-        <v>274</v>
+        <v>386</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B162" t="s">
-        <v>280</v>
+        <v>387</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B163" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B164" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B165" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B168" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B169" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B170" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B171" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B173" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B174" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B183" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B184" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="B185" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B191" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C191">
         <v>3</v>
@@ -3089,10 +3089,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B192" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C192">
         <v>8</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C193">
         <v>5</v>
@@ -3111,10 +3111,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hint system for overworld (need to fill in the actual hints), made hotspot ping more obvious for retards.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A19B825-2532-49B1-BDCC-4E29C1C6D433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758E4D3B-EFDA-47A5-B8B5-4E33AF2B61AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="2775" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3795" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="395">
   <si>
     <t>Key</t>
   </si>
@@ -1190,6 +1190,21 @@
   </si>
   <si>
     <t>overworld_1_temp_intro_0</t>
+  </si>
+  <si>
+    <t>overworld_1_hint</t>
+  </si>
+  <si>
+    <t>test test test</t>
+  </si>
+  <si>
+    <t>overworld_2_hint</t>
+  </si>
+  <si>
+    <t>overworld_3_hint</t>
+  </si>
+  <si>
+    <t>overworld_4_hint</t>
   </si>
 </sst>
 </file>
@@ -1536,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2339,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>177</v>
       </c>
@@ -2332,7 +2347,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>178</v>
       </c>
@@ -2340,7 +2355,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>344</v>
       </c>
@@ -2348,7 +2363,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>180</v>
       </c>
@@ -2356,7 +2371,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>181</v>
       </c>
@@ -2364,7 +2379,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>347</v>
       </c>
@@ -2372,7 +2387,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>348</v>
       </c>
@@ -2380,7 +2395,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>182</v>
       </c>
@@ -2388,7 +2403,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>183</v>
       </c>
@@ -2396,7 +2411,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>184</v>
       </c>
@@ -2404,7 +2419,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>352</v>
       </c>
@@ -2412,7 +2427,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>185</v>
       </c>
@@ -2420,7 +2435,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>188</v>
       </c>
@@ -2428,692 +2443,736 @@
         <v>187</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>390</v>
+      </c>
+      <c r="B110" t="s">
+        <v>391</v>
+      </c>
+      <c r="C110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>189</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>190</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>193</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>195</v>
-      </c>
-      <c r="B113" t="s">
-        <v>198</v>
+        <v>193</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B115" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B116" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B117" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>204</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
+      </c>
+      <c r="B118" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>207</v>
-      </c>
-      <c r="B119" t="s">
-        <v>211</v>
+        <v>204</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B120" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>209</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+      <c r="B121" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>210</v>
-      </c>
-      <c r="B122" t="s">
-        <v>236</v>
+        <v>209</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B124" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B125" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B126" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B127" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B128" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>221</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
+      </c>
+      <c r="B129" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>225</v>
-      </c>
-      <c r="B131" t="s">
-        <v>228</v>
+        <v>222</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>226</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>382</v>
+        <v>225</v>
+      </c>
+      <c r="B132" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>227</v>
-      </c>
-      <c r="B133" t="s">
-        <v>242</v>
+        <v>226</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B134" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B135" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B136" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B137" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B138" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B139" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>362</v>
+        <v>245</v>
       </c>
       <c r="B140" t="s">
-        <v>360</v>
+        <v>246</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B141" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>364</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
+      </c>
+      <c r="B142" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>247</v>
-      </c>
-      <c r="B143" t="s">
-        <v>366</v>
+        <v>364</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>247</v>
+      </c>
+      <c r="B144" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>358</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B145" s="3" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>359</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>365</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>368</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B148" s="3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>370</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B149" s="3" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>371</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B150" s="3" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>248</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>249</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B152" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>250</v>
       </c>
-      <c r="B152" s="3" t="s">
+      <c r="B153" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>392</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>253</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B155" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>254</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B156" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>255</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B157" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>258</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B158" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>259</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B159" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>260</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>264</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B161" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>265</v>
       </c>
-      <c r="B160" s="3" t="s">
+      <c r="B162" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>266</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B163" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>268</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B164" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>269</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>270</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>271</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B167" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>272</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B168" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>277</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B169" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>278</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B170" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>281</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B171" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>282</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B172" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>283</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B173" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>393</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C174">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>287</v>
       </c>
-      <c r="B172" s="3" t="s">
+      <c r="B175" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>288</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B176" t="s">
         <v>290</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>291</v>
-      </c>
-      <c r="B174" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>292</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>295</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>297</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>299</v>
+        <v>291</v>
+      </c>
+      <c r="B177" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>309</v>
-      </c>
-      <c r="B183" t="s">
-        <v>311</v>
+        <v>302</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>310</v>
-      </c>
-      <c r="B184" t="s">
-        <v>312</v>
+        <v>305</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>313</v>
-      </c>
-      <c r="B185" t="s">
-        <v>316</v>
+        <v>306</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>314</v>
+        <v>394</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>338</v>
+        <v>391</v>
+      </c>
+      <c r="C186">
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>315</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>317</v>
+        <v>309</v>
+      </c>
+      <c r="B187" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>318</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>321</v>
+        <v>310</v>
+      </c>
+      <c r="B188" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>319</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>322</v>
+        <v>313</v>
+      </c>
+      <c r="B189" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>329</v>
-      </c>
-      <c r="B191" t="s">
-        <v>331</v>
-      </c>
-      <c r="C191">
-        <v>3</v>
+        <v>315</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>324</v>
-      </c>
-      <c r="B192" t="s">
-        <v>330</v>
-      </c>
-      <c r="C192">
-        <v>8</v>
+        <v>318</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C193">
-        <v>5</v>
+        <v>322</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>320</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>329</v>
+      </c>
+      <c r="B195" t="s">
+        <v>331</v>
+      </c>
+      <c r="C195">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>324</v>
+      </c>
+      <c r="B196" t="s">
+        <v>330</v>
+      </c>
+      <c r="C196">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>325</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>327</v>
       </c>
-      <c r="B194" s="3" t="s">
+      <c r="B198" s="3" t="s">
         <v>328</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjusted tutorials, remove cycle pausing when house is ready (redo text), some UI adjustments for better player feedback.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758E4D3B-EFDA-47A5-B8B5-4E33AF2B61AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E36E61-B8C8-4DF1-9F22-A52AC47F823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3795" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,9 +283,6 @@
     <t>Homes Deployed</t>
   </si>
   <si>
-    <t>A new house is available! Deploy it to progress.</t>
-  </si>
-  <si>
     <t>weather_sunny</t>
   </si>
   <si>
@@ -688,15 +685,9 @@
     <t>colony_1_engineer_placed_1</t>
   </si>
   <si>
-    <t>colony_1_engineer_placed_2</t>
-  </si>
-  <si>
     <t>That’s pretty much it! Remember to keep an eye out for each house’s needs as the population grows.</t>
   </si>
   <si>
-    <t>If you’re feeling confident, you can speed up time by pressing on the ‘play’ button found in the upper right corner of the screen.</t>
-  </si>
-  <si>
     <t>colony_1_vine_0</t>
   </si>
   <si>
@@ -1205,6 +1196,15 @@
   </si>
   <si>
     <t>overworld_4_hint</t>
+  </si>
+  <si>
+    <t>A new house is available! Place it to increase the population!</t>
+  </si>
+  <si>
+    <t>fastforward_hint</t>
+  </si>
+  <si>
+    <t>Press this button if you want to speed up the game.</t>
   </si>
 </sst>
 </file>
@@ -1553,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,7 +1584,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1653,18 +1653,18 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1693,21 +1693,21 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>336</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>338</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>341</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -1747,15 +1747,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -1779,31 +1782,31 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>351</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>353</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>356</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1893,50 +1896,50 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1957,74 +1960,74 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>128</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2101,354 +2104,354 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>103</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>105</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>107</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>109</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B82" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B84" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87" t="s">
         <v>160</v>
-      </c>
-      <c r="B87" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>163</v>
+      </c>
+      <c r="B88" t="s">
         <v>164</v>
-      </c>
-      <c r="B88" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>165</v>
+      </c>
+      <c r="B89" t="s">
         <v>166</v>
-      </c>
-      <c r="B89" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>167</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>169</v>
+      </c>
+      <c r="B91" t="s">
         <v>170</v>
-      </c>
-      <c r="B91" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>171</v>
+      </c>
+      <c r="B92" t="s">
         <v>172</v>
-      </c>
-      <c r="B92" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B93" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>174</v>
+      </c>
+      <c r="B95" t="s">
         <v>175</v>
-      </c>
-      <c r="B95" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B96" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B99" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B101" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>344</v>
+      </c>
+      <c r="B102" t="s">
         <v>347</v>
-      </c>
-      <c r="B102" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>345</v>
+      </c>
+      <c r="B103" t="s">
         <v>348</v>
-      </c>
-      <c r="B103" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B104" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B105" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>184</v>
+      </c>
+      <c r="B108" t="s">
         <v>185</v>
-      </c>
-      <c r="B108" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B109" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B110" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C110">
         <v>5</v>
@@ -2456,354 +2459,357 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B111" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B112" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>192</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B114" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B115" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B116" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B117" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B118" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B120" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B121" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B123" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B124" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B125" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B126" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B127" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B128" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>219</v>
+      </c>
+      <c r="B129" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>220</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>393</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>222</v>
+      </c>
+      <c r="B132" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>223</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>224</v>
+      </c>
+      <c r="B134" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>226</v>
+      </c>
+      <c r="B135" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>220</v>
-      </c>
-      <c r="B129" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>227</v>
+      </c>
+      <c r="B136" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>228</v>
+      </c>
+      <c r="B137" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>229</v>
+      </c>
+      <c r="B138" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>221</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>222</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>225</v>
-      </c>
-      <c r="B132" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>226</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>227</v>
-      </c>
-      <c r="B134" t="s">
+      <c r="B139" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>229</v>
-      </c>
-      <c r="B135" t="s">
+      <c r="B140" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>230</v>
-      </c>
-      <c r="B136" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>231</v>
-      </c>
-      <c r="B137" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>232</v>
-      </c>
-      <c r="B138" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>359</v>
+      </c>
+      <c r="B141" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>360</v>
+      </c>
+      <c r="B142" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>361</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>244</v>
       </c>
-      <c r="B139" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>245</v>
-      </c>
-      <c r="B140" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>362</v>
-      </c>
-      <c r="B141" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="B144" t="s">
         <v>363</v>
-      </c>
-      <c r="B142" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>364</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>247</v>
-      </c>
-      <c r="B144" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B146" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B151" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C154">
         <v>5</v>
@@ -2811,162 +2817,162 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B155" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B156" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B157" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>255</v>
+      </c>
+      <c r="B158" t="s">
         <v>258</v>
-      </c>
-      <c r="B158" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>256</v>
+      </c>
+      <c r="B159" t="s">
         <v>259</v>
-      </c>
-      <c r="B159" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>257</v>
+      </c>
+      <c r="B160" t="s">
         <v>260</v>
-      </c>
-      <c r="B160" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B161" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B163" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B164" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B165" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B166" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B167" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B170" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>278</v>
+      </c>
+      <c r="B171" t="s">
         <v>281</v>
-      </c>
-      <c r="B171" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>279</v>
+      </c>
+      <c r="B172" t="s">
         <v>282</v>
-      </c>
-      <c r="B172" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>280</v>
+      </c>
+      <c r="B173" t="s">
         <v>283</v>
-      </c>
-      <c r="B173" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C174">
         <v>5</v>
@@ -2974,98 +2980,98 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B176" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B177" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C186">
         <v>5</v>
@@ -3073,74 +3079,74 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B187" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B188" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>310</v>
+      </c>
+      <c r="B189" t="s">
         <v>313</v>
-      </c>
-      <c r="B189" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>315</v>
+      </c>
+      <c r="B192" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>316</v>
+      </c>
+      <c r="B193" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>317</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B195" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C195">
         <v>3</v>
@@ -3148,10 +3154,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B196" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C196">
         <v>8</v>
@@ -3159,10 +3165,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C197">
         <v>5</v>
@@ -3170,10 +3176,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added overworld hint texts
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E36E61-B8C8-4DF1-9F22-A52AC47F823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E50EF51-9C5F-442C-AC6D-7F700E501FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3795" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="398">
   <si>
     <t>Key</t>
   </si>
@@ -1186,9 +1186,6 @@
     <t>overworld_1_hint</t>
   </si>
   <si>
-    <t>test test test</t>
-  </si>
-  <si>
     <t>overworld_2_hint</t>
   </si>
   <si>
@@ -1205,6 +1202,18 @@
   </si>
   <si>
     <t>Press this button if you want to speed up the game.</t>
+  </si>
+  <si>
+    <t>In a region with temperate climate, the highest temperature and humidity tends to be during summer.</t>
+  </si>
+  <si>
+    <t>You’re certain to find strong winds in a tropical region during autumn in the Pacific Ocean.</t>
+  </si>
+  <si>
+    <t>Northern Africa is a good desert region for these frogs. Just make sure to pick a season that’s not too hot!</t>
+  </si>
+  <si>
+    <t>We want a mountainous area for this one. How about in South America during summer, when it is cool?</t>
   </si>
 </sst>
 </file>
@@ -1553,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,7 +1761,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -2451,10 +2460,10 @@
         <v>387</v>
       </c>
       <c r="B110" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C110">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2619,10 +2628,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>392</v>
+      </c>
+      <c r="B131" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>394</v>
       </c>
       <c r="C131">
         <v>5</v>
@@ -2806,13 +2815,13 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C154">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2969,13 +2978,13 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="C174">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3068,13 +3077,13 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>391</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>388</v>
+        <v>390</v>
+      </c>
+      <c r="B186" t="s">
+        <v>397</v>
       </c>
       <c r="C186">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adjusted some texts to be more 'simple'. Changed explanation of humidity.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E50EF51-9C5F-442C-AC6D-7F700E501FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2801D655-7873-4117-B75B-656006DAC2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3795" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2625" yWindow="3375" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -493,9 +493,6 @@
     <t>They appear to be frog-like. Let me put on my frog suit to communicate with these peculiar creatures!</t>
   </si>
   <si>
-    <t>Well, why not? Let’s give these hapless frogs some proper homes to settle in. There’s still plenty of room here on Earth.</t>
-  </si>
-  <si>
     <t>Now commencing operation: Project Bloom – A quest for home!</t>
   </si>
   <si>
@@ -628,15 +625,9 @@
     <t>colony_1_post_intro_1</t>
   </si>
   <si>
-    <t>Our goal for this expedition is to populate the place with as many frogs as possible. We do this by deploying houses.</t>
-  </si>
-  <si>
     <t>colony_1_post_intro_2</t>
   </si>
   <si>
-    <t>You can deploy a house by pressing the ‘home’ icon below, then pressing the ‘house’ that appears above it.</t>
-  </si>
-  <si>
     <t>Go ahead and place one in a suitable location.</t>
   </si>
   <si>
@@ -1015,9 +1006,6 @@
     <t>Looks like the temperature is too low. We will need to change when to land on this spot.</t>
   </si>
   <si>
-    <t>Well, we can’t just let them hang about in outer space. Besides, it’s not often we are visited by sentient beings, and frogs no less!</t>
-  </si>
-  <si>
     <t>On the lefthand side of the map are the latitude values. This is the angular distance relative to the earth’s equator.</t>
   </si>
   <si>
@@ -1042,15 +1030,9 @@
     <t>AWAITING ANALYSIS</t>
   </si>
   <si>
-    <t>Notice how humidity tends to be higher near the equator? This coincides with the temperature being high, allowing air to hold more water.</t>
-  </si>
-  <si>
     <t>overworld_1_humid_2</t>
   </si>
   <si>
-    <t>It’s no wonder there is an abundance of trees in these regions!</t>
-  </si>
-  <si>
     <t>Now go ahead and find a place for the frogs to land. Simply press on the map to find the hotspot.</t>
   </si>
   <si>
@@ -1060,9 +1042,6 @@
     <t>overworld_1_hotspot_found_1</t>
   </si>
   <si>
-    <t>Next is the humidity readings of Earth. The percentage tells us the amount of water vapor in the air relative to its capacity based on the current temperature.</t>
-  </si>
-  <si>
     <t>Now that you have found the hotspot, you’ll need to analyze its temperature and humidity readings.</t>
   </si>
   <si>
@@ -1214,6 +1193,27 @@
   </si>
   <si>
     <t>We want a mountainous area for this one. How about in South America during summer, when it is cool?</t>
+  </si>
+  <si>
+    <t>Well, we can’t just let them hang about in outer space. Besides, it’s not often we are visited by space frogs!</t>
+  </si>
+  <si>
+    <t>Well, why not? Let’s give these frogs some proper homes to settle in. There’s still plenty of room here on Earth.</t>
+  </si>
+  <si>
+    <t>Our goal for this expedition is to populate the land with as many frogs as possible. We do this by placing houses.</t>
+  </si>
+  <si>
+    <t>You can place a house by pressing the ‘home’ icon below, then pressing the ‘house’ that appears above it.</t>
+  </si>
+  <si>
+    <t>Next is the humidity readings of Earth.</t>
+  </si>
+  <si>
+    <t>Humidity tells us how much water vapor is in the air. These water vapor comes from evaporation, and is dropped to new location as the air cools down.</t>
+  </si>
+  <si>
+    <t>What you see on the map is the relative humidity in percentage. This is the amount of water in the air relative to the maximum amount of water vapor (moisture).</t>
   </si>
 </sst>
 </file>
@@ -1562,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1601,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1702,18 +1702,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1761,7 +1761,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1793,26 +1793,26 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2236,7 +2236,7 @@
         <v>151</v>
       </c>
       <c r="B82" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>152</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>331</v>
+        <v>391</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2252,7 +2252,7 @@
         <v>153</v>
       </c>
       <c r="B84" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2260,7 +2260,7 @@
         <v>154</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>157</v>
+        <v>392</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2268,199 +2268,199 @@
         <v>155</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>158</v>
+      </c>
+      <c r="B87" t="s">
         <v>159</v>
-      </c>
-      <c r="B87" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>162</v>
+      </c>
+      <c r="B88" t="s">
         <v>163</v>
-      </c>
-      <c r="B88" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>164</v>
+      </c>
+      <c r="B89" t="s">
         <v>165</v>
-      </c>
-      <c r="B89" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>166</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" t="s">
         <v>169</v>
-      </c>
-      <c r="B91" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>170</v>
+      </c>
+      <c r="B92" t="s">
         <v>171</v>
-      </c>
-      <c r="B92" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="B93" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B94" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>173</v>
+      </c>
+      <c r="B95" t="s">
         <v>174</v>
-      </c>
-      <c r="B95" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B96" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>346</v>
+        <v>395</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B98" t="s">
-        <v>340</v>
+        <v>396</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B99" t="s">
-        <v>342</v>
+        <v>397</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B102" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B103" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B104" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B105" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>183</v>
+      </c>
+      <c r="B108" t="s">
         <v>184</v>
-      </c>
-      <c r="B108" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B109" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>380</v>
+      </c>
+      <c r="B110" t="s">
         <v>387</v>
-      </c>
-      <c r="B110" t="s">
-        <v>394</v>
       </c>
       <c r="C110">
         <v>10</v>
@@ -2468,170 +2468,170 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B111" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B112" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>191</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B114" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B115" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B116" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>200</v>
-      </c>
-      <c r="B117" t="s">
-        <v>202</v>
+        <v>199</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B118" t="s">
-        <v>204</v>
+        <v>394</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B120" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B121" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B123" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B124" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B125" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B126" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B127" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B128" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B129" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="C131">
         <v>5</v>
@@ -2639,186 +2639,186 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>219</v>
+      </c>
+      <c r="B132" t="s">
         <v>222</v>
-      </c>
-      <c r="B132" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B134" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B135" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>224</v>
+      </c>
+      <c r="B136" t="s">
         <v>227</v>
-      </c>
-      <c r="B136" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>225</v>
+      </c>
+      <c r="B137" t="s">
         <v>228</v>
-      </c>
-      <c r="B137" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>226</v>
+      </c>
+      <c r="B138" t="s">
         <v>229</v>
-      </c>
-      <c r="B138" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B139" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B140" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="B141" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="B142" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B144" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="B146" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B151" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>381</v>
+      </c>
+      <c r="B154" s="3" t="s">
         <v>388</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>395</v>
       </c>
       <c r="C154">
         <v>10</v>
@@ -2826,162 +2826,162 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B155" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B156" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B157" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>252</v>
+      </c>
+      <c r="B158" t="s">
         <v>255</v>
-      </c>
-      <c r="B158" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>253</v>
+      </c>
+      <c r="B159" t="s">
         <v>256</v>
-      </c>
-      <c r="B159" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>254</v>
+      </c>
+      <c r="B160" t="s">
         <v>257</v>
-      </c>
-      <c r="B160" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B161" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B163" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B164" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B165" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B166" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B167" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B170" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>275</v>
+      </c>
+      <c r="B171" t="s">
         <v>278</v>
-      </c>
-      <c r="B171" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>276</v>
+      </c>
+      <c r="B172" t="s">
         <v>279</v>
-      </c>
-      <c r="B172" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>277</v>
+      </c>
+      <c r="B173" t="s">
         <v>280</v>
-      </c>
-      <c r="B173" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>382</v>
+      </c>
+      <c r="B174" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>396</v>
       </c>
       <c r="C174">
         <v>10</v>
@@ -2989,98 +2989,98 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B176" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B177" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
+        <v>383</v>
+      </c>
+      <c r="B186" t="s">
         <v>390</v>
-      </c>
-      <c r="B186" t="s">
-        <v>397</v>
       </c>
       <c r="C186">
         <v>10</v>
@@ -3088,74 +3088,74 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B187" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B188" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>307</v>
+      </c>
+      <c r="B189" t="s">
         <v>310</v>
-      </c>
-      <c r="B189" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>312</v>
+      </c>
+      <c r="B192" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>313</v>
+      </c>
+      <c r="B193" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>314</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B195" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C195">
         <v>3</v>
@@ -3163,10 +3163,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B196" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C196">
         <v>8</v>
@@ -3174,10 +3174,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C197">
         <v>5</v>
@@ -3185,10 +3185,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overworld 1 gameplay revision complete
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2801D655-7873-4117-B75B-656006DAC2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5856CF3B-CFE2-44E1-8E59-AA355735B5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="3375" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39510" yWindow="2265" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="416">
   <si>
     <t>Key</t>
   </si>
@@ -1214,6 +1214,60 @@
   </si>
   <si>
     <t>What you see on the map is the relative humidity in percentage. This is the amount of water in the air relative to the maximum amount of water vapor (moisture).</t>
+  </si>
+  <si>
+    <t>topographyFeatures</t>
+  </si>
+  <si>
+    <t>topography_forest</t>
+  </si>
+  <si>
+    <t>topography_jungle</t>
+  </si>
+  <si>
+    <t>topography_lake</t>
+  </si>
+  <si>
+    <t>topography_ocean</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Jungle</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>Topographic Features</t>
+  </si>
+  <si>
+    <t>topography_river</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>topography_mountain</t>
+  </si>
+  <si>
+    <t>topography_hill</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>Vegetation</t>
+  </si>
+  <si>
+    <t>topography_vegetation</t>
   </si>
 </sst>
 </file>
@@ -1560,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D198"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,1377 +1871,1449 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>398</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>51</v>
+        <v>407</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>410</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>412</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>411</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>23</v>
+        <v>413</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>399</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>25</v>
+        <v>403</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>400</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>27</v>
+        <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>415</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>414</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>408</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>31</v>
+        <v>409</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>401</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>33</v>
+        <v>405</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>402</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>35</v>
+        <v>406</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>117</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>134</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>131</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>42</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>138</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>38</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>148</v>
-      </c>
-      <c r="B79" t="s">
-        <v>146</v>
+        <v>97</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>149</v>
-      </c>
-      <c r="B80" t="s">
-        <v>156</v>
+        <v>93</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>150</v>
-      </c>
-      <c r="B81" t="s">
-        <v>147</v>
+        <v>95</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>151</v>
-      </c>
-      <c r="B82" t="s">
-        <v>368</v>
+        <v>101</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>152</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>391</v>
+        <v>99</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>153</v>
-      </c>
-      <c r="B84" t="s">
-        <v>369</v>
+        <v>103</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>154</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>392</v>
+        <v>105</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>155</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>157</v>
+        <v>107</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>158</v>
-      </c>
-      <c r="B87" t="s">
-        <v>159</v>
+        <v>109</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B88" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B89" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>166</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>167</v>
+        <v>150</v>
+      </c>
+      <c r="B90" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B91" t="s">
-        <v>169</v>
+        <v>368</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>170</v>
-      </c>
-      <c r="B92" t="s">
-        <v>171</v>
+        <v>152</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>378</v>
+        <v>153</v>
       </c>
       <c r="B93" t="s">
-        <v>328</v>
+        <v>369</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>379</v>
-      </c>
-      <c r="B94" t="s">
-        <v>172</v>
+        <v>154</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>173</v>
-      </c>
-      <c r="B95" t="s">
-        <v>174</v>
+        <v>155</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>158</v>
+      </c>
+      <c r="B96" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>162</v>
+      </c>
+      <c r="B97" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>164</v>
+      </c>
+      <c r="B98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>166</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>168</v>
+      </c>
+      <c r="B100" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>170</v>
+      </c>
+      <c r="B101" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>378</v>
+      </c>
+      <c r="B102" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>379</v>
+      </c>
+      <c r="B103" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>173</v>
+      </c>
+      <c r="B104" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>329</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B105" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>175</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B106" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>176</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B107" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>336</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B108" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>178</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>179</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>338</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B111" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>339</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B112" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>180</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B113" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>181</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B114" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>182</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>342</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>183</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B117" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>186</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B118" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>380</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B119" t="s">
         <v>387</v>
       </c>
-      <c r="C110">
+      <c r="C119">
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>187</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B120" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>188</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B121" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>191</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>193</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B123" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>194</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B124" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>195</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B125" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>199</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B126" s="3" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>200</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B127" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>201</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B128" s="3" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>203</v>
-      </c>
-      <c r="B120" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>204</v>
-      </c>
-      <c r="B121" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>205</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>206</v>
-      </c>
-      <c r="B123" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>210</v>
-      </c>
-      <c r="B124" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>211</v>
-      </c>
-      <c r="B125" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>212</v>
-      </c>
-      <c r="B126" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>213</v>
-      </c>
-      <c r="B127" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>214</v>
-      </c>
-      <c r="B128" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="B129" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>217</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>218</v>
+        <v>204</v>
+      </c>
+      <c r="B130" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>385</v>
+        <v>205</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="C131">
-        <v>5</v>
+        <v>209</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="B132" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>220</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>372</v>
+        <v>210</v>
+      </c>
+      <c r="B133" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B134" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B135" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="B136" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B137" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B138" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>238</v>
-      </c>
-      <c r="B139" t="s">
-        <v>246</v>
+        <v>217</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>239</v>
-      </c>
-      <c r="B140" t="s">
-        <v>240</v>
+        <v>385</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C140">
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>352</v>
+        <v>219</v>
       </c>
       <c r="B141" t="s">
-        <v>350</v>
+        <v>222</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>353</v>
-      </c>
-      <c r="B142" t="s">
-        <v>364</v>
+        <v>220</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>354</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>351</v>
+        <v>221</v>
+      </c>
+      <c r="B143" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>223</v>
+      </c>
+      <c r="B144" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>224</v>
+      </c>
+      <c r="B145" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>225</v>
+      </c>
+      <c r="B146" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>226</v>
+      </c>
+      <c r="B147" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>238</v>
+      </c>
+      <c r="B148" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>239</v>
+      </c>
+      <c r="B149" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>352</v>
+      </c>
+      <c r="B150" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>353</v>
+      </c>
+      <c r="B151" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>354</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>241</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B153" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>348</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="B154" s="3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>349</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B155" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>355</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>358</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B157" s="3" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>360</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B158" s="3" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>361</v>
       </c>
-      <c r="B150" s="3" t="s">
+      <c r="B159" s="3" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>242</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B160" t="s">
         <v>366</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>243</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>244</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>381</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C154">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>247</v>
-      </c>
-      <c r="B155" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>248</v>
-      </c>
-      <c r="B156" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>249</v>
-      </c>
-      <c r="B157" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>252</v>
-      </c>
-      <c r="B158" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>253</v>
-      </c>
-      <c r="B159" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>254</v>
-      </c>
-      <c r="B160" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>258</v>
-      </c>
-      <c r="B161" t="s">
-        <v>375</v>
+        <v>243</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>261</v>
+        <v>373</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>260</v>
-      </c>
-      <c r="B163" t="s">
-        <v>376</v>
+        <v>381</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C163">
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="B164" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="B165" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B166" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="B167" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>266</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>270</v>
+        <v>253</v>
+      </c>
+      <c r="B168" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>271</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>273</v>
+        <v>254</v>
+      </c>
+      <c r="B169" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B170" t="s">
-        <v>274</v>
+        <v>375</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>275</v>
-      </c>
-      <c r="B171" t="s">
-        <v>278</v>
+        <v>259</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="B172" t="s">
-        <v>279</v>
+        <v>376</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="B173" t="s">
-        <v>280</v>
+        <v>377</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>382</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C174">
-        <v>10</v>
+        <v>263</v>
+      </c>
+      <c r="B174" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>281</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>283</v>
+        <v>264</v>
+      </c>
+      <c r="B175" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="B176" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>285</v>
-      </c>
-      <c r="B177" t="s">
-        <v>287</v>
+        <v>266</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>289</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>290</v>
+        <v>272</v>
+      </c>
+      <c r="B179" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>291</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>293</v>
+        <v>275</v>
+      </c>
+      <c r="B180" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>292</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>294</v>
+        <v>276</v>
+      </c>
+      <c r="B181" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>295</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>297</v>
+        <v>277</v>
+      </c>
+      <c r="B182" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>296</v>
+        <v>382</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>298</v>
+        <v>389</v>
+      </c>
+      <c r="C183">
+        <v>10</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>300</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
+      </c>
+      <c r="B185" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>383</v>
+        <v>285</v>
       </c>
       <c r="B186" t="s">
-        <v>390</v>
-      </c>
-      <c r="C186">
-        <v>10</v>
+        <v>287</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>303</v>
-      </c>
-      <c r="B187" t="s">
-        <v>305</v>
+        <v>286</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>304</v>
-      </c>
-      <c r="B188" t="s">
-        <v>306</v>
+        <v>289</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>307</v>
-      </c>
-      <c r="B189" t="s">
-        <v>310</v>
+        <v>291</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>331</v>
+        <v>294</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>323</v>
+        <v>383</v>
       </c>
       <c r="B195" t="s">
-        <v>325</v>
+        <v>390</v>
       </c>
       <c r="C195">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="B196" t="s">
-        <v>324</v>
-      </c>
-      <c r="C196">
-        <v>8</v>
+        <v>305</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>319</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C197">
-        <v>5</v>
+        <v>304</v>
+      </c>
+      <c r="B197" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>307</v>
+      </c>
+      <c r="B198" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>308</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>309</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>312</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>313</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>314</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>323</v>
+      </c>
+      <c r="B204" t="s">
+        <v>325</v>
+      </c>
+      <c r="C204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>318</v>
+      </c>
+      <c r="B205" t="s">
+        <v>324</v>
+      </c>
+      <c r="C205">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>319</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C206">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>321</v>
       </c>
-      <c r="B198" s="3" t="s">
+      <c r="B207" s="3" t="s">
         <v>322</v>
       </c>
     </row>

</xml_diff>

<commit_message>
colony 02 revise initial complete pass, various tweaks/fixes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5856CF3B-CFE2-44E1-8E59-AA355735B5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878D94B2-B7B4-4890-B065-7D453BFD06E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39510" yWindow="2265" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="2310" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="418">
   <si>
     <t>Key</t>
   </si>
@@ -1000,9 +1000,6 @@
     <t>CONGRATULATIONS</t>
   </si>
   <si>
-    <t>RENEGADEWARE 2023</t>
-  </si>
-  <si>
     <t>Looks like the temperature is too low. We will need to change when to land on this spot.</t>
   </si>
   <si>
@@ -1268,6 +1265,15 @@
   </si>
   <si>
     <t>topography_vegetation</t>
+  </si>
+  <si>
+    <t>RENEGADEWARE</t>
+  </si>
+  <si>
+    <t>warning</t>
+  </si>
+  <si>
+    <t>WARNING</t>
   </si>
 </sst>
 </file>
@@ -1614,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1661,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>326</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,18 +1762,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>331</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>333</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1815,7 +1821,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1855,1465 +1861,1473 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>343</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>345</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>407</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>416</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>51</v>
+        <v>417</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>148</v>
-      </c>
-      <c r="B88" t="s">
-        <v>146</v>
+        <v>109</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B89" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B90" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B91" t="s">
-        <v>368</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>152</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>391</v>
+        <v>151</v>
+      </c>
+      <c r="B92" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>153</v>
-      </c>
-      <c r="B93" t="s">
-        <v>369</v>
+        <v>152</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>154</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>392</v>
+        <v>153</v>
+      </c>
+      <c r="B94" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>157</v>
+        <v>391</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>158</v>
-      </c>
-      <c r="B96" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B97" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B98" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>166</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B99" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>168</v>
-      </c>
-      <c r="B100" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B101" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>378</v>
+        <v>170</v>
       </c>
       <c r="B102" t="s">
-        <v>328</v>
+        <v>171</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B103" t="s">
-        <v>172</v>
+        <v>327</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>173</v>
+        <v>378</v>
       </c>
       <c r="B104" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>329</v>
+        <v>173</v>
       </c>
       <c r="B105" t="s">
-        <v>330</v>
+        <v>174</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>175</v>
+        <v>328</v>
       </c>
       <c r="B106" t="s">
-        <v>395</v>
+        <v>329</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B107" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>336</v>
+        <v>176</v>
       </c>
       <c r="B108" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>178</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
+      </c>
+      <c r="B109" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>179</v>
-      </c>
-      <c r="B110" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>338</v>
+        <v>179</v>
       </c>
       <c r="B111" t="s">
-        <v>340</v>
+        <v>177</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>337</v>
+      </c>
+      <c r="B112" t="s">
         <v>339</v>
-      </c>
-      <c r="B112" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>180</v>
+        <v>338</v>
       </c>
       <c r="B113" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B114" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>182</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>371</v>
+        <v>181</v>
+      </c>
+      <c r="B115" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>342</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>343</v>
+        <v>182</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>183</v>
-      </c>
-      <c r="B117" t="s">
-        <v>184</v>
+        <v>341</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B118" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>380</v>
+        <v>186</v>
       </c>
       <c r="B119" t="s">
-        <v>387</v>
-      </c>
-      <c r="C119">
-        <v>10</v>
+        <v>185</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>187</v>
+        <v>379</v>
       </c>
       <c r="B120" t="s">
-        <v>189</v>
+        <v>386</v>
+      </c>
+      <c r="C120">
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B121" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>191</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="B122" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>193</v>
-      </c>
-      <c r="B123" t="s">
-        <v>196</v>
+        <v>191</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B124" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B125" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>199</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>393</v>
+        <v>195</v>
+      </c>
+      <c r="B126" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>200</v>
-      </c>
-      <c r="B127" t="s">
-        <v>394</v>
+        <v>199</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>201</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="B128" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>203</v>
-      </c>
-      <c r="B129" t="s">
-        <v>207</v>
+        <v>201</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B130" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>205</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+      <c r="B131" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>206</v>
-      </c>
-      <c r="B132" t="s">
-        <v>230</v>
+        <v>205</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B133" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B134" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B135" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B136" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B137" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B138" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>217</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
+      </c>
+      <c r="B139" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>385</v>
+        <v>217</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="C140">
-        <v>5</v>
+        <v>218</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>219</v>
-      </c>
-      <c r="B141" t="s">
-        <v>222</v>
+        <v>384</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>220</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>372</v>
+        <v>219</v>
+      </c>
+      <c r="B142" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>221</v>
-      </c>
-      <c r="B143" t="s">
-        <v>236</v>
+        <v>220</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B144" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B145" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B146" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B147" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B148" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B149" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>352</v>
+        <v>239</v>
       </c>
       <c r="B150" t="s">
-        <v>350</v>
+        <v>240</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B151" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>354</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
+      </c>
+      <c r="B152" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>241</v>
-      </c>
-      <c r="B153" t="s">
-        <v>356</v>
+        <v>353</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>348</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>357</v>
+        <v>241</v>
+      </c>
+      <c r="B154" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>349</v>
-      </c>
-      <c r="B155" t="s">
-        <v>365</v>
+        <v>347</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>355</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>367</v>
+        <v>348</v>
+      </c>
+      <c r="B156" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>358</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>359</v>
+      </c>
+      <c r="B159" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>242</v>
-      </c>
-      <c r="B160" t="s">
-        <v>366</v>
+        <v>360</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>243</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
+      </c>
+      <c r="B161" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>373</v>
+        <v>245</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>381</v>
+        <v>244</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C163">
-        <v>10</v>
+        <v>372</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>247</v>
-      </c>
-      <c r="B164" t="s">
-        <v>374</v>
+        <v>380</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C164">
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B165" t="s">
-        <v>250</v>
+        <v>373</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B166" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B167" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B168" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B169" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B170" t="s">
-        <v>375</v>
+        <v>257</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>259</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
+      </c>
+      <c r="B171" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>260</v>
-      </c>
-      <c r="B172" t="s">
-        <v>376</v>
+        <v>259</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B173" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B174" t="s">
-        <v>267</v>
+        <v>376</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B175" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B176" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>266</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
+      </c>
+      <c r="B177" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>272</v>
-      </c>
-      <c r="B179" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B180" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B181" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B182" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>382</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C183">
-        <v>10</v>
+        <v>277</v>
+      </c>
+      <c r="B183" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>281</v>
+        <v>381</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>283</v>
+        <v>388</v>
+      </c>
+      <c r="C184">
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>282</v>
-      </c>
-      <c r="B185" t="s">
-        <v>284</v>
+        <v>281</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B186" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>286</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
+      </c>
+      <c r="B187" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>383</v>
-      </c>
-      <c r="B195" t="s">
-        <v>390</v>
-      </c>
-      <c r="C195">
-        <v>10</v>
+        <v>300</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>303</v>
+        <v>382</v>
       </c>
       <c r="B196" t="s">
-        <v>305</v>
+        <v>389</v>
+      </c>
+      <c r="C196">
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B197" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B198" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>308</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>331</v>
+        <v>307</v>
+      </c>
+      <c r="B199" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>323</v>
-      </c>
-      <c r="B204" t="s">
-        <v>325</v>
-      </c>
-      <c r="C204">
-        <v>3</v>
+        <v>314</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="B205" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C205">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>319</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
+      </c>
+      <c r="B206" t="s">
+        <v>324</v>
       </c>
       <c r="C206">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>319</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C207">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>321</v>
       </c>
-      <c r="B207" s="3" t="s">
+      <c r="B208" s="3" t="s">
         <v>322</v>
       </c>
     </row>

</xml_diff>

<commit_message>
colony 4 revised, added snow storm weather
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878D94B2-B7B4-4890-B065-7D453BFD06E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28FE27F-FEE8-4D89-8A4B-B6285F143684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6570" yWindow="2310" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="420">
   <si>
     <t>Key</t>
   </si>
@@ -1274,6 +1274,12 @@
   </si>
   <si>
     <t>WARNING</t>
+  </si>
+  <si>
+    <t>weather_snow_storm</t>
+  </si>
+  <si>
+    <t>Snow Storm</t>
   </si>
 </sst>
 </file>
@@ -1620,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D208"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,985 +2355,993 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>148</v>
-      </c>
-      <c r="B89" t="s">
-        <v>146</v>
+        <v>418</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B90" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B91" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B92" t="s">
-        <v>367</v>
+        <v>147</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>152</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>390</v>
+        <v>151</v>
+      </c>
+      <c r="B93" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>153</v>
-      </c>
-      <c r="B94" t="s">
-        <v>368</v>
+        <v>152</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>154</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>391</v>
+        <v>153</v>
+      </c>
+      <c r="B95" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>157</v>
+        <v>391</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>158</v>
-      </c>
-      <c r="B97" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B98" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B99" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>166</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B100" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>168</v>
-      </c>
-      <c r="B101" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B102" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>377</v>
+        <v>170</v>
       </c>
       <c r="B103" t="s">
-        <v>327</v>
+        <v>171</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B104" t="s">
-        <v>172</v>
+        <v>327</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>173</v>
+        <v>378</v>
       </c>
       <c r="B105" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>328</v>
+        <v>173</v>
       </c>
       <c r="B106" t="s">
-        <v>329</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>175</v>
+        <v>328</v>
       </c>
       <c r="B107" t="s">
-        <v>394</v>
+        <v>329</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B108" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>335</v>
+        <v>176</v>
       </c>
       <c r="B109" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>178</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="B110" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>179</v>
-      </c>
-      <c r="B111" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>337</v>
+        <v>179</v>
       </c>
       <c r="B112" t="s">
-        <v>339</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B113" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>180</v>
+        <v>338</v>
       </c>
       <c r="B114" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B115" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>182</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>370</v>
+        <v>181</v>
+      </c>
+      <c r="B116" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>341</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>342</v>
+        <v>182</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>183</v>
-      </c>
-      <c r="B118" t="s">
-        <v>184</v>
+        <v>341</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B119" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>379</v>
+        <v>186</v>
       </c>
       <c r="B120" t="s">
-        <v>386</v>
-      </c>
-      <c r="C120">
-        <v>10</v>
+        <v>185</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>187</v>
+        <v>379</v>
       </c>
       <c r="B121" t="s">
-        <v>189</v>
+        <v>386</v>
+      </c>
+      <c r="C121">
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B122" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>191</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="B123" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>193</v>
-      </c>
-      <c r="B124" t="s">
-        <v>196</v>
+        <v>191</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B125" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B126" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>199</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>392</v>
+        <v>195</v>
+      </c>
+      <c r="B127" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>200</v>
-      </c>
-      <c r="B128" t="s">
-        <v>393</v>
+        <v>199</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>201</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="B129" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>203</v>
-      </c>
-      <c r="B130" t="s">
-        <v>207</v>
+        <v>201</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B131" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>205</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+      <c r="B132" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>206</v>
-      </c>
-      <c r="B133" t="s">
-        <v>230</v>
+        <v>205</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B134" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B135" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B136" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B137" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B138" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B139" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>217</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
+      </c>
+      <c r="B140" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>384</v>
+        <v>217</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C141">
-        <v>5</v>
+        <v>218</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>219</v>
-      </c>
-      <c r="B142" t="s">
-        <v>222</v>
+        <v>384</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C142">
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>220</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>371</v>
+        <v>219</v>
+      </c>
+      <c r="B143" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>221</v>
-      </c>
-      <c r="B144" t="s">
-        <v>236</v>
+        <v>220</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B145" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B146" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B147" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B148" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B149" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B150" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>351</v>
+        <v>239</v>
       </c>
       <c r="B151" t="s">
-        <v>349</v>
+        <v>240</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B152" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>353</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
+      </c>
+      <c r="B153" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>241</v>
-      </c>
-      <c r="B154" t="s">
-        <v>355</v>
+        <v>353</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>347</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>356</v>
+        <v>241</v>
+      </c>
+      <c r="B155" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>348</v>
-      </c>
-      <c r="B156" t="s">
-        <v>364</v>
+        <v>347</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>354</v>
-      </c>
-      <c r="B157" s="4" t="s">
-        <v>366</v>
+        <v>348</v>
+      </c>
+      <c r="B157" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>357</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>242</v>
-      </c>
-      <c r="B161" t="s">
-        <v>365</v>
+        <v>360</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>243</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
+      </c>
+      <c r="B162" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>372</v>
+        <v>245</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>380</v>
+        <v>244</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="C164">
-        <v>10</v>
+        <v>372</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>247</v>
-      </c>
-      <c r="B165" t="s">
-        <v>373</v>
+        <v>380</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C165">
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B166" t="s">
-        <v>250</v>
+        <v>373</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B167" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B168" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B169" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B170" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B171" t="s">
-        <v>374</v>
+        <v>257</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>259</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
+      </c>
+      <c r="B172" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>260</v>
-      </c>
-      <c r="B173" t="s">
-        <v>375</v>
+        <v>259</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B174" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B175" t="s">
-        <v>267</v>
+        <v>376</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B176" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B177" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>266</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
+      </c>
+      <c r="B178" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>272</v>
-      </c>
-      <c r="B180" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B181" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B182" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B183" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>381</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C184">
-        <v>10</v>
+        <v>277</v>
+      </c>
+      <c r="B184" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>281</v>
+        <v>381</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>283</v>
+        <v>388</v>
+      </c>
+      <c r="C185">
+        <v>10</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>282</v>
-      </c>
-      <c r="B186" t="s">
-        <v>284</v>
+        <v>281</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B187" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>286</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
+      </c>
+      <c r="B188" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>382</v>
-      </c>
-      <c r="B196" t="s">
-        <v>389</v>
-      </c>
-      <c r="C196">
-        <v>10</v>
+        <v>300</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>303</v>
+        <v>382</v>
       </c>
       <c r="B197" t="s">
-        <v>305</v>
+        <v>389</v>
+      </c>
+      <c r="C197">
+        <v>10</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B198" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B199" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>308</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>330</v>
+        <v>307</v>
+      </c>
+      <c r="B200" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>323</v>
-      </c>
-      <c r="B205" t="s">
-        <v>325</v>
-      </c>
-      <c r="C205">
-        <v>3</v>
+        <v>314</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="B206" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C206">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>319</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
+      </c>
+      <c r="B207" t="s">
+        <v>324</v>
       </c>
       <c r="C207">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>319</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C208">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>321</v>
       </c>
-      <c r="B208" s="3" t="s">
+      <c r="B209" s="3" t="s">
         <v>322</v>
       </c>
     </row>

</xml_diff>

<commit_message>
colony 04 revision initial complete, overworld 2 revision topography maps added
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28FE27F-FEE8-4D89-8A4B-B6285F143684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92819774-215A-46F3-9784-591255CA6299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6570" yWindow="2310" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="422">
   <si>
     <t>Key</t>
   </si>
@@ -1280,6 +1280,12 @@
   </si>
   <si>
     <t>Snow Storm</t>
+  </si>
+  <si>
+    <t>topography_swamp</t>
+  </si>
+  <si>
+    <t>Swamp</t>
   </si>
 </sst>
 </file>
@@ -1626,10 +1632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,1393 +1961,1401 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>416</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>51</v>
+        <v>417</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>418</v>
+        <v>109</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>419</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>148</v>
-      </c>
-      <c r="B90" t="s">
-        <v>146</v>
+        <v>418</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B91" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B92" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B93" t="s">
-        <v>367</v>
+        <v>147</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>152</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>390</v>
+        <v>151</v>
+      </c>
+      <c r="B94" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>153</v>
-      </c>
-      <c r="B95" t="s">
-        <v>368</v>
+        <v>152</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>154</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>391</v>
+        <v>153</v>
+      </c>
+      <c r="B96" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>157</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>158</v>
-      </c>
-      <c r="B98" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B99" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B100" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>166</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B101" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>168</v>
-      </c>
-      <c r="B102" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B103" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>377</v>
+        <v>170</v>
       </c>
       <c r="B104" t="s">
-        <v>327</v>
+        <v>171</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B105" t="s">
-        <v>172</v>
+        <v>327</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>173</v>
+        <v>378</v>
       </c>
       <c r="B106" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>328</v>
+        <v>173</v>
       </c>
       <c r="B107" t="s">
-        <v>329</v>
+        <v>174</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>175</v>
+        <v>328</v>
       </c>
       <c r="B108" t="s">
-        <v>394</v>
+        <v>329</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B109" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>335</v>
+        <v>176</v>
       </c>
       <c r="B110" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>178</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="B111" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>179</v>
-      </c>
-      <c r="B112" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>337</v>
+        <v>179</v>
       </c>
       <c r="B113" t="s">
-        <v>339</v>
+        <v>177</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B114" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>180</v>
+        <v>338</v>
       </c>
       <c r="B115" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B116" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>182</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>370</v>
+        <v>181</v>
+      </c>
+      <c r="B117" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>341</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>342</v>
+        <v>182</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>183</v>
-      </c>
-      <c r="B119" t="s">
-        <v>184</v>
+        <v>341</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B120" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>379</v>
+        <v>186</v>
       </c>
       <c r="B121" t="s">
-        <v>386</v>
-      </c>
-      <c r="C121">
-        <v>10</v>
+        <v>185</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>187</v>
+        <v>379</v>
       </c>
       <c r="B122" t="s">
-        <v>189</v>
+        <v>386</v>
+      </c>
+      <c r="C122">
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B123" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>191</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="B124" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>193</v>
-      </c>
-      <c r="B125" t="s">
-        <v>196</v>
+        <v>191</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B126" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B127" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>199</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>392</v>
+        <v>195</v>
+      </c>
+      <c r="B128" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>200</v>
-      </c>
-      <c r="B129" t="s">
-        <v>393</v>
+        <v>199</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>201</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="B130" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>203</v>
-      </c>
-      <c r="B131" t="s">
-        <v>207</v>
+        <v>201</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B132" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>205</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+      <c r="B133" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>206</v>
-      </c>
-      <c r="B134" t="s">
-        <v>230</v>
+        <v>205</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B135" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B136" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B137" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B138" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B139" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B140" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>217</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
+      </c>
+      <c r="B141" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>384</v>
+        <v>217</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C142">
-        <v>5</v>
+        <v>218</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>219</v>
-      </c>
-      <c r="B143" t="s">
-        <v>222</v>
+        <v>384</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C143">
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>220</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>371</v>
+        <v>219</v>
+      </c>
+      <c r="B144" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>221</v>
-      </c>
-      <c r="B145" t="s">
-        <v>236</v>
+        <v>220</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B146" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B147" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B148" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B149" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B150" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B151" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>351</v>
+        <v>239</v>
       </c>
       <c r="B152" t="s">
-        <v>349</v>
+        <v>240</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B153" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>353</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
+      </c>
+      <c r="B154" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>241</v>
-      </c>
-      <c r="B155" t="s">
-        <v>355</v>
+        <v>353</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>347</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>356</v>
+        <v>241</v>
+      </c>
+      <c r="B156" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>348</v>
-      </c>
-      <c r="B157" t="s">
-        <v>364</v>
+        <v>347</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>354</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>366</v>
+        <v>348</v>
+      </c>
+      <c r="B158" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>357</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>242</v>
-      </c>
-      <c r="B162" t="s">
-        <v>365</v>
+        <v>360</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>243</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
+      </c>
+      <c r="B163" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>372</v>
+        <v>245</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>380</v>
+        <v>244</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="C165">
-        <v>10</v>
+        <v>372</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>247</v>
-      </c>
-      <c r="B166" t="s">
-        <v>373</v>
+        <v>380</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C166">
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B167" t="s">
-        <v>250</v>
+        <v>373</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B168" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B169" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B170" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B171" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B172" t="s">
-        <v>374</v>
+        <v>257</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>259</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
+      </c>
+      <c r="B173" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>260</v>
-      </c>
-      <c r="B174" t="s">
-        <v>375</v>
+        <v>259</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B175" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B176" t="s">
-        <v>267</v>
+        <v>376</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B177" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B178" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>266</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
+      </c>
+      <c r="B179" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>272</v>
-      </c>
-      <c r="B181" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B182" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B183" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B184" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>381</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C185">
-        <v>10</v>
+        <v>277</v>
+      </c>
+      <c r="B185" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>281</v>
+        <v>381</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>283</v>
+        <v>388</v>
+      </c>
+      <c r="C186">
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>282</v>
-      </c>
-      <c r="B187" t="s">
-        <v>284</v>
+        <v>281</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B188" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>286</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
+      </c>
+      <c r="B189" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>382</v>
-      </c>
-      <c r="B197" t="s">
-        <v>389</v>
-      </c>
-      <c r="C197">
-        <v>10</v>
+        <v>300</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>303</v>
+        <v>382</v>
       </c>
       <c r="B198" t="s">
-        <v>305</v>
+        <v>389</v>
+      </c>
+      <c r="C198">
+        <v>10</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B199" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B200" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>308</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>330</v>
+        <v>307</v>
+      </c>
+      <c r="B201" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>323</v>
-      </c>
-      <c r="B206" t="s">
-        <v>325</v>
-      </c>
-      <c r="C206">
-        <v>3</v>
+        <v>314</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="B207" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C207">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>318</v>
+      </c>
+      <c r="B208" t="s">
+        <v>324</v>
+      </c>
+      <c r="C208">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>319</v>
       </c>
-      <c r="B208" s="3" t="s">
+      <c r="B209" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="C208">
+      <c r="C209">
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>321</v>
       </c>
-      <c r="B209" s="3" t="s">
+      <c r="B210" s="3" t="s">
         <v>322</v>
       </c>
     </row>

</xml_diff>

<commit_message>
overworld 03 revision stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92819774-215A-46F3-9784-591255CA6299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E473E40-3599-45FC-A309-8EF0FDD79B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6570" yWindow="2310" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="424">
   <si>
     <t>Key</t>
   </si>
@@ -1286,6 +1286,12 @@
   </si>
   <si>
     <t>Swamp</t>
+  </si>
+  <si>
+    <t>topography_oasis</t>
+  </si>
+  <si>
+    <t>Oasis</t>
   </si>
 </sst>
 </file>
@@ -1632,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D210"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,1393 +1975,1401 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>416</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>51</v>
+        <v>417</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>418</v>
+        <v>109</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>419</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>148</v>
-      </c>
-      <c r="B91" t="s">
-        <v>146</v>
+        <v>418</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B93" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B94" t="s">
-        <v>367</v>
+        <v>147</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>152</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>390</v>
+        <v>151</v>
+      </c>
+      <c r="B95" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>153</v>
-      </c>
-      <c r="B96" t="s">
-        <v>368</v>
+        <v>152</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>154</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>391</v>
+        <v>153</v>
+      </c>
+      <c r="B97" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>157</v>
+        <v>391</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>158</v>
-      </c>
-      <c r="B99" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B100" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B101" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>166</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B102" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>168</v>
-      </c>
-      <c r="B103" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B104" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>377</v>
+        <v>170</v>
       </c>
       <c r="B105" t="s">
-        <v>327</v>
+        <v>171</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B106" t="s">
-        <v>172</v>
+        <v>327</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>173</v>
+        <v>378</v>
       </c>
       <c r="B107" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>328</v>
+        <v>173</v>
       </c>
       <c r="B108" t="s">
-        <v>329</v>
+        <v>174</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>175</v>
+        <v>328</v>
       </c>
       <c r="B109" t="s">
-        <v>394</v>
+        <v>329</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B110" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>335</v>
+        <v>176</v>
       </c>
       <c r="B111" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>178</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="B112" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>179</v>
-      </c>
-      <c r="B113" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>337</v>
+        <v>179</v>
       </c>
       <c r="B114" t="s">
-        <v>339</v>
+        <v>177</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B115" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>180</v>
+        <v>338</v>
       </c>
       <c r="B116" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B117" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>182</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>370</v>
+        <v>181</v>
+      </c>
+      <c r="B118" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>341</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>342</v>
+        <v>182</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>183</v>
-      </c>
-      <c r="B120" t="s">
-        <v>184</v>
+        <v>341</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B121" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>379</v>
+        <v>186</v>
       </c>
       <c r="B122" t="s">
-        <v>386</v>
-      </c>
-      <c r="C122">
-        <v>10</v>
+        <v>185</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>187</v>
+        <v>379</v>
       </c>
       <c r="B123" t="s">
-        <v>189</v>
+        <v>386</v>
+      </c>
+      <c r="C123">
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B124" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>191</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="B125" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>193</v>
-      </c>
-      <c r="B126" t="s">
-        <v>196</v>
+        <v>191</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B127" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B128" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>199</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>392</v>
+        <v>195</v>
+      </c>
+      <c r="B129" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>200</v>
-      </c>
-      <c r="B130" t="s">
-        <v>393</v>
+        <v>199</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>201</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="B131" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>203</v>
-      </c>
-      <c r="B132" t="s">
-        <v>207</v>
+        <v>201</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B133" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>205</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+      <c r="B134" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>206</v>
-      </c>
-      <c r="B135" t="s">
-        <v>230</v>
+        <v>205</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B136" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B137" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B138" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B139" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B140" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B141" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>217</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
+      </c>
+      <c r="B142" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>384</v>
+        <v>217</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C143">
-        <v>5</v>
+        <v>218</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>219</v>
-      </c>
-      <c r="B144" t="s">
-        <v>222</v>
+        <v>384</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C144">
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>220</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>371</v>
+        <v>219</v>
+      </c>
+      <c r="B145" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>221</v>
-      </c>
-      <c r="B146" t="s">
-        <v>236</v>
+        <v>220</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B147" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B148" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B149" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B150" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B151" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B152" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>351</v>
+        <v>239</v>
       </c>
       <c r="B153" t="s">
-        <v>349</v>
+        <v>240</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B154" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>353</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
+      </c>
+      <c r="B155" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>241</v>
-      </c>
-      <c r="B156" t="s">
-        <v>355</v>
+        <v>353</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>347</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>356</v>
+        <v>241</v>
+      </c>
+      <c r="B157" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>348</v>
-      </c>
-      <c r="B158" t="s">
-        <v>364</v>
+        <v>347</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>354</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>366</v>
+        <v>348</v>
+      </c>
+      <c r="B159" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>357</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>242</v>
-      </c>
-      <c r="B163" t="s">
-        <v>365</v>
+        <v>360</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>243</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
+      </c>
+      <c r="B164" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>372</v>
+        <v>245</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>380</v>
+        <v>244</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="C166">
-        <v>10</v>
+        <v>372</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>247</v>
-      </c>
-      <c r="B167" t="s">
-        <v>373</v>
+        <v>380</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C167">
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B168" t="s">
-        <v>250</v>
+        <v>373</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B169" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B170" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B171" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B172" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B173" t="s">
-        <v>374</v>
+        <v>257</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>259</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
+      </c>
+      <c r="B174" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>260</v>
-      </c>
-      <c r="B175" t="s">
-        <v>375</v>
+        <v>259</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B176" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B177" t="s">
-        <v>267</v>
+        <v>376</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B178" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B179" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>266</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
+      </c>
+      <c r="B180" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>272</v>
-      </c>
-      <c r="B182" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B183" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B184" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B185" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>381</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C186">
-        <v>10</v>
+        <v>277</v>
+      </c>
+      <c r="B186" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>281</v>
+        <v>381</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>283</v>
+        <v>388</v>
+      </c>
+      <c r="C187">
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>282</v>
-      </c>
-      <c r="B188" t="s">
-        <v>284</v>
+        <v>281</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B189" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>286</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
+      </c>
+      <c r="B190" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>382</v>
-      </c>
-      <c r="B198" t="s">
-        <v>389</v>
-      </c>
-      <c r="C198">
-        <v>10</v>
+        <v>300</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>303</v>
+        <v>382</v>
       </c>
       <c r="B199" t="s">
-        <v>305</v>
+        <v>389</v>
+      </c>
+      <c r="C199">
+        <v>10</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B200" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B201" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>308</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>330</v>
+        <v>307</v>
+      </c>
+      <c r="B202" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>323</v>
-      </c>
-      <c r="B207" t="s">
-        <v>325</v>
-      </c>
-      <c r="C207">
-        <v>3</v>
+        <v>314</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="B208" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C208">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>319</v>
-      </c>
-      <c r="B209" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
+      </c>
+      <c r="B209" t="s">
+        <v>324</v>
       </c>
       <c r="C209">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>319</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C210">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>321</v>
       </c>
-      <c r="B210" s="3" t="s">
+      <c r="B211" s="3" t="s">
         <v>322</v>
       </c>
     </row>

</xml_diff>

<commit_message>
overworld 1 and colony 1 lessons/dialogs reworked
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E473E40-3599-45FC-A309-8EF0FDD79B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A61743-6C4B-465A-ACC1-D5439C561087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="2310" windowWidth="27315" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40530" yWindow="1575" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -535,9 +535,6 @@
     <t>overworld_1_criteria_0</t>
   </si>
   <si>
-    <t>In this case, we need to find a place where it’s fairly warm and humid.</t>
-  </si>
-  <si>
     <t>Now let’s view the temperature readings of Earth.</t>
   </si>
   <si>
@@ -547,39 +544,15 @@
     <t>As you can see, the temperature is consistently hot starting from the equator, and gets colder further north or south.</t>
   </si>
   <si>
-    <t>overworld_1_humid_0</t>
-  </si>
-  <si>
-    <t>overworld_1_humid_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remember to make use of the temperature and humidity reading. </t>
-  </si>
-  <si>
     <t>overworld_1_hotspot_0</t>
   </si>
   <si>
     <t>overworld_1_hotspot_1</t>
   </si>
   <si>
-    <t>overworld_1_analyze_0</t>
-  </si>
-  <si>
-    <t>overworld_1_analyze_1</t>
-  </si>
-  <si>
-    <t>overworld_1_analyze_2</t>
-  </si>
-  <si>
     <t>overworld_1_investigate_0</t>
   </si>
   <si>
-    <t>Now you just need to pick a particular location on the land for the frogs.</t>
-  </si>
-  <si>
-    <t>When the majority of the frogs approve, we can finally launch the expedition!</t>
-  </si>
-  <si>
     <t>overworld_1_investigate_1</t>
   </si>
   <si>
@@ -625,117 +598,9 @@
     <t>colony_1_post_intro_1</t>
   </si>
   <si>
-    <t>colony_1_post_intro_2</t>
-  </si>
-  <si>
-    <t>Go ahead and place one in a suitable location.</t>
-  </si>
-  <si>
     <t>colony_1_house_placed_0</t>
   </si>
   <si>
-    <t>colony_1_house_placed_1</t>
-  </si>
-  <si>
-    <t>colony_1_house_placed_2</t>
-  </si>
-  <si>
-    <t>colony_1_house_placed_3</t>
-  </si>
-  <si>
-    <t>Excellent! Now that a house has landed, our population has increased by one!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In order to increase the population further, we are going to need food. These peculiar frogs seem to only eat a certain type of flower that they grow. </t>
-  </si>
-  <si>
-    <t>To grow this flower, you just need to place it somewhere suitable much like you did with the house.</t>
-  </si>
-  <si>
-    <t>colony_1_house_second_0</t>
-  </si>
-  <si>
-    <t>colony_1_house_second_1</t>
-  </si>
-  <si>
-    <t>colony_1_house_second_2</t>
-  </si>
-  <si>
-    <t>colony_1_water_solar_placed_0</t>
-  </si>
-  <si>
-    <t>colony_1_water_solar_placed_1</t>
-  </si>
-  <si>
-    <t>With both the water tank and solar panel placed, you’ll need an engineer to build them.</t>
-  </si>
-  <si>
-    <t>colony_1_engineer_placed_0</t>
-  </si>
-  <si>
-    <t>colony_1_engineer_placed_1</t>
-  </si>
-  <si>
-    <t>That’s pretty much it! Remember to keep an eye out for each house’s needs as the population grows.</t>
-  </si>
-  <si>
-    <t>colony_1_vine_0</t>
-  </si>
-  <si>
-    <t>colony_1_vine_1</t>
-  </si>
-  <si>
-    <t>colony_1_vine_2</t>
-  </si>
-  <si>
-    <t>Watch out! It looks like weeds are starting to grow on one of the structures!</t>
-  </si>
-  <si>
-    <t>colony_1_mole_0</t>
-  </si>
-  <si>
-    <t>colony_1_mole_1</t>
-  </si>
-  <si>
-    <t>colony_1_mole_2</t>
-  </si>
-  <si>
-    <t>colony_1_mole_3</t>
-  </si>
-  <si>
-    <t>You’re going to need a hero frog to deal with these moles!</t>
-  </si>
-  <si>
-    <t>To summon a hero frog, simply click on the funny-looking frog with a red cape when the green arrow appears.</t>
-  </si>
-  <si>
-    <t>If your frog summon bar is full, you can unsummon some of the frogs by pressing on their portrait when the red arrow appears.</t>
-  </si>
-  <si>
-    <t>You’ll then need a gardener to nurture the flower. Simply click on the frog with a hat portrait when the green arrow appears.</t>
-  </si>
-  <si>
-    <t>Now that we have a couple of houses placed, we will now need to sustain them with water and power.</t>
-  </si>
-  <si>
-    <t>To build these structures, simply press on the ‘gear’ icon at the bottom.</t>
-  </si>
-  <si>
-    <t>Press the water tank for water, and press the solar panel for power. Remember to place each of them to proceed!</t>
-  </si>
-  <si>
-    <t>To summon an engineer, press on the frog with a yellow hard helmet portrait when the green arrow appears.</t>
-  </si>
-  <si>
-    <t>The engineer will now proceed to build both the water tank and the solar panel.</t>
-  </si>
-  <si>
-    <t>A gardener should be able to take care of these weeds!</t>
-  </si>
-  <si>
-    <t>A mole! These creatures don’t see very well, so they mistake our structures as something to dig through.</t>
-  </si>
-  <si>
     <t>overworld_2_intro_0</t>
   </si>
   <si>
@@ -1000,9 +865,6 @@
     <t>CONGRATULATIONS</t>
   </si>
   <si>
-    <t>Looks like the temperature is too low. We will need to change when to land on this spot.</t>
-  </si>
-  <si>
     <t>On the lefthand side of the map are the latitude values. This is the angular distance relative to the earth’s equator.</t>
   </si>
   <si>
@@ -1027,30 +889,6 @@
     <t>AWAITING ANALYSIS</t>
   </si>
   <si>
-    <t>overworld_1_humid_2</t>
-  </si>
-  <si>
-    <t>Now go ahead and find a place for the frogs to land. Simply press on the map to find the hotspot.</t>
-  </si>
-  <si>
-    <t>overworld_1_hotspot_found_0</t>
-  </si>
-  <si>
-    <t>overworld_1_hotspot_found_1</t>
-  </si>
-  <si>
-    <t>Now that you have found the hotspot, you’ll need to analyze its temperature and humidity readings.</t>
-  </si>
-  <si>
-    <t>Remember to switch between the temperature and humidity overlay to analyze them both.</t>
-  </si>
-  <si>
-    <t>overworld_1_analyze_3</t>
-  </si>
-  <si>
-    <t>Remember to reanalyze the atmospheric readings when changing seasons.</t>
-  </si>
-  <si>
     <t>lowPressure</t>
   </si>
   <si>
@@ -1129,15 +967,6 @@
     <t>They are expressing their gratitude and are ready to cooperate.</t>
   </si>
   <si>
-    <t>Since the earth rotates at a slightly tilted axis around the Sun, the atmosphere can change throughout the year.</t>
-  </si>
-  <si>
-    <t>Let's adjust the time by selecting a different season. Perhaps summer will give us the temperature to satisfy the criteria!</t>
-  </si>
-  <si>
-    <t>Though the weather is ideal for the frogs, unfortunately, it is also ideal for these invasive plants.</t>
-  </si>
-  <si>
     <t>This time around, there is more than one hotspot to discover on the map. Only one of them will match with the frogs’ criteria.</t>
   </si>
   <si>
@@ -1159,9 +988,6 @@
     <t>overworld_1_temp_intro_0</t>
   </si>
   <si>
-    <t>overworld_1_hint</t>
-  </si>
-  <si>
     <t>overworld_2_hint</t>
   </si>
   <si>
@@ -1180,9 +1006,6 @@
     <t>Press this button if you want to speed up the game.</t>
   </si>
   <si>
-    <t>In a region with temperate climate, the highest temperature and humidity tends to be during summer.</t>
-  </si>
-  <si>
     <t>You’re certain to find strong winds in a tropical region during autumn in the Pacific Ocean.</t>
   </si>
   <si>
@@ -1198,12 +1021,6 @@
     <t>Well, why not? Let’s give these frogs some proper homes to settle in. There’s still plenty of room here on Earth.</t>
   </si>
   <si>
-    <t>Our goal for this expedition is to populate the land with as many frogs as possible. We do this by placing houses.</t>
-  </si>
-  <si>
-    <t>You can place a house by pressing the ‘home’ icon below, then pressing the ‘house’ that appears above it.</t>
-  </si>
-  <si>
     <t>Next is the humidity readings of Earth.</t>
   </si>
   <si>
@@ -1292,6 +1109,189 @@
   </si>
   <si>
     <t>Oasis</t>
+  </si>
+  <si>
+    <t>overworld_2_humid_0</t>
+  </si>
+  <si>
+    <t>overworld_2_humid_1</t>
+  </si>
+  <si>
+    <t>overworld_2_humid_2</t>
+  </si>
+  <si>
+    <t>overworld_1_hotspot_2</t>
+  </si>
+  <si>
+    <t>Use this tool to get a general reading of the Earth’s atmosphere.</t>
+  </si>
+  <si>
+    <t>For now, we have only one spot to investigate.</t>
+  </si>
+  <si>
+    <t>Press the hotspot on the map to continue.</t>
+  </si>
+  <si>
+    <t>In this case, we need to find a place where it’s fairly warm.</t>
+  </si>
+  <si>
+    <t>overworld_1_investigate_intro_0</t>
+  </si>
+  <si>
+    <t>Now we need a suitable area for the frogs to call home.</t>
+  </si>
+  <si>
+    <t>overworld_1_investigate_map_0</t>
+  </si>
+  <si>
+    <t>overworld_1_investigate_map_1</t>
+  </si>
+  <si>
+    <t>overworld_1_investigate_map_2</t>
+  </si>
+  <si>
+    <t>Here’s the topographic map of the land.</t>
+  </si>
+  <si>
+    <t>The atmosphere can vary greatly based on where you live.</t>
+  </si>
+  <si>
+    <t>Be it near the mountains, or alongside a river. Your location can be hotter or colder than normal.</t>
+  </si>
+  <si>
+    <t>overworld_1_investigate_2</t>
+  </si>
+  <si>
+    <t>Now simply press on the map to determine where to place the frog colony.</t>
+  </si>
+  <si>
+    <t>Remember to be mindful of the location’s Altitude and Topographic Features.</t>
+  </si>
+  <si>
+    <t>Once the criteria are met, you will be able to launch the expedition!</t>
+  </si>
+  <si>
+    <t>frog_gardener</t>
+  </si>
+  <si>
+    <t>Gardener</t>
+  </si>
+  <si>
+    <t>frog_engineer</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>frog_hero</t>
+  </si>
+  <si>
+    <t>Fighter</t>
+  </si>
+  <si>
+    <t>colony_1_summon_title</t>
+  </si>
+  <si>
+    <t>Summoning Frogs</t>
+  </si>
+  <si>
+    <t>colony_1_summon_action</t>
+  </si>
+  <si>
+    <t>colony_1_summon_full</t>
+  </si>
+  <si>
+    <t>Full!</t>
+  </si>
+  <si>
+    <t>colony_1_summon_unsummon</t>
+  </si>
+  <si>
+    <t>Summon!</t>
+  </si>
+  <si>
+    <t>Unsummon!</t>
+  </si>
+  <si>
+    <t>Our goal for this expedition is to populate the land with as many frogs as possible.</t>
+  </si>
+  <si>
+    <t>Frog houses will arrive as the population grows.</t>
+  </si>
+  <si>
+    <t>In order to grow the population, we will need to plant crops, build water tanks, and build power stations.</t>
+  </si>
+  <si>
+    <t>colony_1_plant_placed_0</t>
+  </si>
+  <si>
+    <t>colony_1_plant_placed_1</t>
+  </si>
+  <si>
+    <t>colony_1_plant_placed_2</t>
+  </si>
+  <si>
+    <t>Let’s start with plants.</t>
+  </si>
+  <si>
+    <t>We’re going to need a Gardener to help with growing plants.</t>
+  </si>
+  <si>
+    <t>Gardeners can also help with getting rid of weeds, and other sorts of plant-based menace.</t>
+  </si>
+  <si>
+    <t>colony_1_summon_inst_0</t>
+  </si>
+  <si>
+    <t>colony_1_summon_inst_1</t>
+  </si>
+  <si>
+    <t>colony_1_summon_inst_2</t>
+  </si>
+  <si>
+    <t>In order to summon a frog, simply press on their portrait when the green arrow appears.</t>
+  </si>
+  <si>
+    <t>Remember that you can only have a certain number of frogs summoned at a time!</t>
+  </si>
+  <si>
+    <t>If the capacity is full, you can free up a slot by pressing on a frog’s portrait when the red arrow appears.</t>
+  </si>
+  <si>
+    <t>colony_1_water_placed_0</t>
+  </si>
+  <si>
+    <t>colony_1_water_placed_1</t>
+  </si>
+  <si>
+    <t>colony_1_water_placed_2</t>
+  </si>
+  <si>
+    <t>Engineers can also repair structures that are damaged.</t>
+  </si>
+  <si>
+    <t>colony_1_mole_appear_0</t>
+  </si>
+  <si>
+    <t>colony_1_mole_appear_1</t>
+  </si>
+  <si>
+    <t>colony_1_mole_appear_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch out, a mole has appeared! </t>
+  </si>
+  <si>
+    <t>These creatures don’t see very well, so they mistake our structures as something to dig through.</t>
+  </si>
+  <si>
+    <t>Summon a Fighter frog to deal with such pesky creatures!</t>
+  </si>
+  <si>
+    <t>Looks like the frogs are requesting for a construction of a water tank, and a solar panel!</t>
+  </si>
+  <si>
+    <t>Why don’t you summon an Engineer frog to help with these constructions.</t>
   </si>
 </sst>
 </file>
@@ -1640,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,7 +1679,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>415</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,18 +1780,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>331</v>
+        <v>285</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>332</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>333</v>
+        <v>287</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>334</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>383</v>
+        <v>325</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1879,114 +1879,114 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>343</v>
+        <v>289</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>344</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>345</v>
+        <v>291</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>346</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>397</v>
+        <v>336</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>406</v>
+        <v>345</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>409</v>
+        <v>348</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>411</v>
+        <v>350</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>410</v>
+        <v>349</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>412</v>
+        <v>351</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>398</v>
+        <v>337</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>402</v>
+        <v>341</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>399</v>
+        <v>338</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>403</v>
+        <v>342</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>414</v>
+        <v>353</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>413</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>407</v>
+        <v>346</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>408</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>400</v>
+        <v>339</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>404</v>
+        <v>343</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>401</v>
+        <v>340</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>405</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>420</v>
+        <v>359</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>421</v>
+        <v>360</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>422</v>
+        <v>361</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>423</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>416</v>
+        <v>355</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>417</v>
+        <v>356</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2383,624 +2383,621 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>418</v>
+        <v>357</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>419</v>
+        <v>358</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>148</v>
-      </c>
-      <c r="B92" t="s">
-        <v>146</v>
+        <v>383</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>149</v>
-      </c>
-      <c r="B93" t="s">
-        <v>156</v>
+        <v>385</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>150</v>
-      </c>
-      <c r="B94" t="s">
-        <v>147</v>
+        <v>387</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B95" t="s">
-        <v>367</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>152</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>390</v>
+        <v>149</v>
+      </c>
+      <c r="B96" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B97" t="s">
-        <v>368</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>154</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>391</v>
+        <v>151</v>
+      </c>
+      <c r="B98" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>157</v>
+        <v>331</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B100" t="s">
-        <v>159</v>
+        <v>314</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>162</v>
-      </c>
-      <c r="B101" t="s">
-        <v>163</v>
+        <v>154</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>164</v>
-      </c>
-      <c r="B102" t="s">
-        <v>165</v>
+        <v>155</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>166</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
+      </c>
+      <c r="B103" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B104" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B105" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>377</v>
-      </c>
-      <c r="B106" t="s">
-        <v>327</v>
+        <v>166</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>378</v>
+        <v>168</v>
       </c>
       <c r="B107" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B108" t="s">
-        <v>174</v>
+        <v>370</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B109" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>175</v>
+        <v>321</v>
       </c>
       <c r="B110" t="s">
-        <v>394</v>
+        <v>171</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B111" t="s">
-        <v>395</v>
+        <v>173</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>335</v>
+        <v>282</v>
       </c>
       <c r="B112" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>174</v>
+      </c>
+      <c r="B113" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>175</v>
+      </c>
+      <c r="B114" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>366</v>
+      </c>
+      <c r="B115" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>371</v>
+      </c>
+      <c r="B116" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>373</v>
+      </c>
+      <c r="B117" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>374</v>
+      </c>
+      <c r="B118" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>375</v>
+      </c>
+      <c r="B119" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>176</v>
+      </c>
+      <c r="B120" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>177</v>
+      </c>
+      <c r="B121" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>379</v>
+      </c>
+      <c r="B122" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>178</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="B123" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>179</v>
       </c>
-      <c r="B114" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>337</v>
-      </c>
-      <c r="B115" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>338</v>
-      </c>
-      <c r="B116" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>180</v>
-      </c>
-      <c r="B117" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="B124" t="s">
         <v>181</v>
       </c>
-      <c r="B118" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>182</v>
       </c>
-      <c r="B119" s="3" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>341</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="B125" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B121" t="s">
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="B126" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>185</v>
+      </c>
+      <c r="B127" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>186</v>
       </c>
-      <c r="B122" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>379</v>
-      </c>
-      <c r="B123" t="s">
-        <v>386</v>
-      </c>
-      <c r="C123">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>187</v>
-      </c>
-      <c r="B124" t="s">
+      <c r="B128" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>188</v>
-      </c>
-      <c r="B125" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>191</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>193</v>
-      </c>
-      <c r="B127" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>194</v>
-      </c>
-      <c r="B128" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>195</v>
+        <v>389</v>
       </c>
       <c r="B129" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>199</v>
-      </c>
-      <c r="B130" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B130" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>392</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>200</v>
       </c>
       <c r="B131" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>394</v>
+      </c>
+      <c r="B132" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>190</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>191</v>
+      </c>
+      <c r="B134" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>192</v>
+      </c>
+      <c r="B135" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>400</v>
+      </c>
+      <c r="B136" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>401</v>
+      </c>
+      <c r="B137" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>402</v>
+      </c>
+      <c r="B138" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>406</v>
+      </c>
+      <c r="B139" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>407</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>408</v>
+      </c>
+      <c r="B141" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>412</v>
+      </c>
+      <c r="B142" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>413</v>
+      </c>
+      <c r="B143" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>414</v>
+      </c>
+      <c r="B144" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>416</v>
+      </c>
+      <c r="B145" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>417</v>
+      </c>
+      <c r="B146" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>418</v>
+      </c>
+      <c r="B147" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>326</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C148">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>193</v>
+      </c>
+      <c r="B149" t="s">
         <v>201</v>
       </c>
-      <c r="B132" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>203</v>
-      </c>
-      <c r="B133" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>204</v>
-      </c>
-      <c r="B134" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>205</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>206</v>
-      </c>
-      <c r="B136" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>210</v>
-      </c>
-      <c r="B137" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>211</v>
-      </c>
-      <c r="B138" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>212</v>
-      </c>
-      <c r="B139" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>213</v>
-      </c>
-      <c r="B140" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>214</v>
-      </c>
-      <c r="B141" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>216</v>
-      </c>
-      <c r="B142" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>217</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>384</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="C144">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>219</v>
-      </c>
-      <c r="B145" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>220</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>221</v>
-      </c>
-      <c r="B147" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>223</v>
-      </c>
-      <c r="B148" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>224</v>
-      </c>
-      <c r="B149" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="B150" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>226</v>
+        <v>363</v>
       </c>
       <c r="B151" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>238</v>
+        <v>364</v>
       </c>
       <c r="B152" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>239</v>
+        <v>365</v>
       </c>
       <c r="B153" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>351</v>
+        <v>297</v>
       </c>
       <c r="B154" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>352</v>
+        <v>298</v>
       </c>
       <c r="B155" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>353</v>
+        <v>299</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>241</v>
+        <v>196</v>
       </c>
       <c r="B157" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>347</v>
+        <v>293</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>348</v>
+        <v>294</v>
       </c>
       <c r="B159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>354</v>
+        <v>300</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>366</v>
+        <v>312</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>357</v>
+        <v>303</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>358</v>
+        <v>304</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>359</v>
+        <v>305</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>361</v>
+        <v>307</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>360</v>
+        <v>306</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>362</v>
+        <v>308</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="B164" t="s">
-        <v>365</v>
+        <v>311</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>372</v>
+        <v>315</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>380</v>
+        <v>322</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>387</v>
+        <v>328</v>
       </c>
       <c r="C167">
         <v>10</v>
@@ -3008,162 +3005,162 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>247</v>
+        <v>202</v>
       </c>
       <c r="B168" t="s">
-        <v>373</v>
+        <v>316</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>248</v>
+        <v>203</v>
       </c>
       <c r="B169" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>249</v>
+        <v>204</v>
       </c>
       <c r="B170" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="B171" t="s">
-        <v>255</v>
+        <v>210</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>253</v>
+        <v>208</v>
       </c>
       <c r="B172" t="s">
-        <v>256</v>
+        <v>211</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>254</v>
+        <v>209</v>
       </c>
       <c r="B173" t="s">
-        <v>257</v>
+        <v>212</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="B174" t="s">
-        <v>374</v>
+        <v>317</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>261</v>
+        <v>216</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="B176" t="s">
-        <v>375</v>
+        <v>318</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>262</v>
+        <v>217</v>
       </c>
       <c r="B177" t="s">
-        <v>376</v>
+        <v>319</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="B178" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="B179" t="s">
-        <v>268</v>
+        <v>223</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="B180" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>270</v>
+        <v>225</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>272</v>
+        <v>227</v>
       </c>
       <c r="B183" t="s">
-        <v>274</v>
+        <v>229</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="B184" t="s">
-        <v>278</v>
+        <v>233</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
       <c r="B185" t="s">
-        <v>279</v>
+        <v>234</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="B186" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>381</v>
+        <v>323</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>388</v>
+        <v>329</v>
       </c>
       <c r="C187">
         <v>10</v>
@@ -3171,98 +3168,98 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="B189" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="B190" t="s">
-        <v>287</v>
+        <v>242</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>286</v>
+        <v>241</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>288</v>
+        <v>243</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>290</v>
+        <v>245</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>291</v>
+        <v>246</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>293</v>
+        <v>248</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>292</v>
+        <v>247</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>294</v>
+        <v>249</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>295</v>
+        <v>250</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>297</v>
+        <v>252</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>296</v>
+        <v>251</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>298</v>
+        <v>253</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>299</v>
+        <v>254</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>301</v>
+        <v>256</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>300</v>
+        <v>255</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>382</v>
+        <v>324</v>
       </c>
       <c r="B199" t="s">
-        <v>389</v>
+        <v>330</v>
       </c>
       <c r="C199">
         <v>10</v>
@@ -3270,74 +3267,74 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="B200" t="s">
-        <v>305</v>
+        <v>260</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>304</v>
+        <v>259</v>
       </c>
       <c r="B201" t="s">
-        <v>306</v>
+        <v>261</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>307</v>
+        <v>262</v>
       </c>
       <c r="B202" t="s">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>308</v>
+        <v>263</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>330</v>
+        <v>284</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>309</v>
+        <v>264</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>311</v>
+        <v>266</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>312</v>
+        <v>267</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>315</v>
+        <v>270</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>313</v>
+        <v>268</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>316</v>
+        <v>271</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>314</v>
+        <v>269</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>317</v>
+        <v>272</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>323</v>
+        <v>278</v>
       </c>
       <c r="B208" t="s">
-        <v>325</v>
+        <v>280</v>
       </c>
       <c r="C208">
         <v>3</v>
@@ -3345,10 +3342,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>318</v>
+        <v>273</v>
       </c>
       <c r="B209" t="s">
-        <v>324</v>
+        <v>279</v>
       </c>
       <c r="C209">
         <v>8</v>
@@ -3356,10 +3353,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>319</v>
+        <v>274</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>320</v>
+        <v>275</v>
       </c>
       <c r="C210">
         <v>5</v>
@@ -3367,10 +3364,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>322</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overworld 2 and colony 2 lesson stuff revised
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A61743-6C4B-465A-ACC1-D5439C561087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB718DC-5647-461C-B140-5C5DB8980243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40530" yWindow="1575" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42225" yWindow="1485" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="418">
   <si>
     <t>Key</t>
   </si>
@@ -607,99 +607,21 @@
     <t>overworld_2_intro_1</t>
   </si>
   <si>
-    <t>In that case, we’ll need to check the wind readings of Earth.</t>
-  </si>
-  <si>
-    <t>overworld_2_wind_0</t>
-  </si>
-  <si>
     <t>overworld_2_post_intro_0</t>
   </si>
   <si>
     <t>overworld_2_post_intro_1</t>
   </si>
   <si>
-    <t>overworld_2_post_intro_2</t>
-  </si>
-  <si>
-    <t>Remember to check the different seasons to see how the wind changes to various positions across Earth.</t>
-  </si>
-  <si>
-    <t>Our next batch of frogs are keen on living in a windy environment, as well as hot and humid.</t>
-  </si>
-  <si>
     <t>colony_2_intro_0</t>
   </si>
   <si>
     <t>colony_2_intro_1</t>
   </si>
   <si>
-    <t>colony_2_intro_2</t>
-  </si>
-  <si>
     <t>Though it looks like we’re getting more rain than usual, something is afoot...</t>
   </si>
   <si>
-    <t>Perhaps we should take a careful look at the weather forecast.</t>
-  </si>
-  <si>
-    <t>colony_2_mushroom_0</t>
-  </si>
-  <si>
-    <t>colony_2_mushroom_1</t>
-  </si>
-  <si>
-    <t>colony_2_mushroom_2</t>
-  </si>
-  <si>
-    <t>Uh oh, a mushroom has grown near one of our structures!</t>
-  </si>
-  <si>
-    <t>Since there's a lot of moisture in the region, the fungi that grow these mushrooms are able to absorb a lot of nutrients.</t>
-  </si>
-  <si>
-    <t>Their spores appear to be harmful to the frogs! Make sure to have a gardener around to take care of them!</t>
-  </si>
-  <si>
-    <t>colony_2_fly_0</t>
-  </si>
-  <si>
-    <t>colony_2_fly_1</t>
-  </si>
-  <si>
-    <t>colony_2_fly_2</t>
-  </si>
-  <si>
-    <t>Due to the consistent warmth in tropical climates, insects are able to thrive throughout the year.</t>
-  </si>
-  <si>
-    <t>colony_2_hazzard_0</t>
-  </si>
-  <si>
-    <t>colony_2_hazzard_1</t>
-  </si>
-  <si>
-    <t>colony_2_hazzard_2</t>
-  </si>
-  <si>
-    <t>colony_2_hazzard_3</t>
-  </si>
-  <si>
-    <t>colony_2_hazzard_4</t>
-  </si>
-  <si>
-    <t>As mentioned before about hurricanes: the wind speed that has accumulated over low pressure from the surface has reached critical speed.</t>
-  </si>
-  <si>
-    <t>Our frogs must take cover. Fortunately, their structures are made of sturdy stuff, causing it to withstand the staggering winds!</t>
-  </si>
-  <si>
-    <t>However, along with strong winds, the water that is released from the storm will cause flood across the land.</t>
-  </si>
-  <si>
-    <t>Make certain that no important structures are within the flooding area, or they will get damaged.</t>
-  </si>
-  <si>
     <t>overworld_3_intro_0</t>
   </si>
   <si>
@@ -901,48 +823,21 @@
     <t>High Pressure</t>
   </si>
   <si>
-    <t>overworld_2_wind_1</t>
-  </si>
-  <si>
-    <t>overworld_2_wind_2</t>
-  </si>
-  <si>
     <t>Notice how the winds tend to travel diagonally across Earth? This is due to the Coriolis effect.</t>
   </si>
   <si>
     <t>Let’s take a look again on the map.</t>
   </si>
   <si>
-    <t>overworld_2_coriolis_0</t>
-  </si>
-  <si>
-    <t>overworld_2_coriolis_1</t>
-  </si>
-  <si>
-    <t>overworld_2_coriolis_2</t>
-  </si>
-  <si>
-    <t>overworld_2_wind_3</t>
-  </si>
-  <si>
     <t>These are the general directions of the global winds. As warm air from the equator rises up, it cools down and sinks towards north or south.</t>
   </si>
   <si>
     <t>Sometimes, interactions between the low- and high-pressure winds will cause a cyclone, such as the ones you see on the map.</t>
   </si>
   <si>
-    <t>overworld_2_ocean_0</t>
-  </si>
-  <si>
     <t>One other thing to note is how the wind drives the surface ocean currents, which help regulates the temperature across the lands.</t>
   </si>
   <si>
-    <t>overworld_2_gulf_stream_0</t>
-  </si>
-  <si>
-    <t>overworld_2_gulf_stream_1</t>
-  </si>
-  <si>
     <t>Here is an example of an ocean current that brings warm water from the equator towards north, known as the Gulf Stream.</t>
   </si>
   <si>
@@ -955,9 +850,6 @@
     <t>These cyclones can become dangerous as it accumulates wind speed and heavy amounts of water, as it travels across the land.</t>
   </si>
   <si>
-    <t>Anyhow, let’s find places where the wind might be strong. Try looking for areas prone to hurricanes, or typhoons along coastal regions.</t>
-  </si>
-  <si>
     <t>These are often called hurricanes in the Atlantic Ocean, and typhoons in the Pacific Ocean.</t>
   </si>
   <si>
@@ -967,30 +859,15 @@
     <t>They are expressing their gratitude and are ready to cooperate.</t>
   </si>
   <si>
-    <t>This time around, there is more than one hotspot to discover on the map. Only one of them will match with the frogs’ criteria.</t>
-  </si>
-  <si>
     <t>Looks like we’ve landed in a tropical climate, where it’s hot and humid all year round with plenty of rain.</t>
   </si>
   <si>
-    <t>Look out! It's a beetle!</t>
-  </si>
-  <si>
-    <t>These troublesome insects can be dealt with by a hero frog. Make sure to have one around to get them out.</t>
-  </si>
-  <si>
-    <t>Take cover! A hurricane is heading our way!</t>
-  </si>
-  <si>
     <t>overworld_1_latitude_0</t>
   </si>
   <si>
     <t>overworld_1_temp_intro_0</t>
   </si>
   <si>
-    <t>overworld_2_hint</t>
-  </si>
-  <si>
     <t>overworld_3_hint</t>
   </si>
   <si>
@@ -1006,9 +883,6 @@
     <t>Press this button if you want to speed up the game.</t>
   </si>
   <si>
-    <t>You’re certain to find strong winds in a tropical region during autumn in the Pacific Ocean.</t>
-  </si>
-  <si>
     <t>Northern Africa is a good desert region for these frogs. Just make sure to pick a season that’s not too hot!</t>
   </si>
   <si>
@@ -1021,9 +895,6 @@
     <t>Well, why not? Let’s give these frogs some proper homes to settle in. There’s still plenty of room here on Earth.</t>
   </si>
   <si>
-    <t>Next is the humidity readings of Earth.</t>
-  </si>
-  <si>
     <t>Humidity tells us how much water vapor is in the air. These water vapor comes from evaporation, and is dropped to new location as the air cools down.</t>
   </si>
   <si>
@@ -1117,9 +988,6 @@
     <t>overworld_2_humid_1</t>
   </si>
   <si>
-    <t>overworld_2_humid_2</t>
-  </si>
-  <si>
     <t>overworld_1_hotspot_2</t>
   </si>
   <si>
@@ -1292,6 +1160,120 @@
   </si>
   <si>
     <t>Why don’t you summon an Engineer frog to help with these constructions.</t>
+  </si>
+  <si>
+    <t>overworld_3_coriolis_0</t>
+  </si>
+  <si>
+    <t>overworld_3_coriolis_1</t>
+  </si>
+  <si>
+    <t>overworld_3_coriolis_2</t>
+  </si>
+  <si>
+    <t>overworld_3_wind_0</t>
+  </si>
+  <si>
+    <t>overworld_3_wind_1</t>
+  </si>
+  <si>
+    <t>overworld_3_wind_2</t>
+  </si>
+  <si>
+    <t>overworld_3_wind_3</t>
+  </si>
+  <si>
+    <t>overworld_3_ocean_0</t>
+  </si>
+  <si>
+    <t>overworld_3_gulf_stream_0</t>
+  </si>
+  <si>
+    <t>overworld_3_gulf_stream_1</t>
+  </si>
+  <si>
+    <t>Our next batch of frogs are keen on living in a hot and humid environment.</t>
+  </si>
+  <si>
+    <t>Since we already know about temperature, why don’t we learn a bit about humidity.</t>
+  </si>
+  <si>
+    <t>This time around, there are more than one hotspot to investigate on the map.</t>
+  </si>
+  <si>
+    <t>Make good use of the temperature and humidity readings to decide which hotspots are worthy of investigation.</t>
+  </si>
+  <si>
+    <t>weather_cyclone</t>
+  </si>
+  <si>
+    <t>Cyclone</t>
+  </si>
+  <si>
+    <t>colony_2_storm_intro_0</t>
+  </si>
+  <si>
+    <t>Uh oh, looks like a storm is starting to form.</t>
+  </si>
+  <si>
+    <t>colony_2_storm_explain_0</t>
+  </si>
+  <si>
+    <t>colony_2_storm_explain_1</t>
+  </si>
+  <si>
+    <t>Due to the hot temperature of the water, warm air is starting to rise up above the sky.</t>
+  </si>
+  <si>
+    <t>As high-pressure air starts to fill in the low-pressure air from the center, more and more moisture starts to accumulate upwards.</t>
+  </si>
+  <si>
+    <t>colony_2_storm_power_0</t>
+  </si>
+  <si>
+    <t>colony_2_storm_power_1</t>
+  </si>
+  <si>
+    <t>With so much moisture condensing up above, huge clouds start to form.</t>
+  </si>
+  <si>
+    <t>colony_2_storm_end_0</t>
+  </si>
+  <si>
+    <t>colony_2_storm_end_1</t>
+  </si>
+  <si>
+    <t>Fortunately, as the storm moves towards the land, it will no longer have enough warm moisture to sustain its form.</t>
+  </si>
+  <si>
+    <t>structure_wind_transform</t>
+  </si>
+  <si>
+    <t>Wind Turbine Defense</t>
+  </si>
+  <si>
+    <t>colony_2_wind_defense_0</t>
+  </si>
+  <si>
+    <t>colony_2_wind_defense_1</t>
+  </si>
+  <si>
+    <t>colony_2_wind_defense_intro_0</t>
+  </si>
+  <si>
+    <t>Look out! A debris is about to crash into the colony!</t>
+  </si>
+  <si>
+    <t>Luckily our wind turbines come equip with the ability to thwart their destruction!</t>
+  </si>
+  <si>
+    <t>Simply press any of the wind turbines to transform them into a windy shield.</t>
+  </si>
+  <si>
+    <t>And with that much heat circulating, its power continuously grows into epic proportion!</t>
+  </si>
+  <si>
+    <t>Though the storm may have weakened, it is still strong enough to cause wanton destruction along its path!</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1358,6 +1340,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1638,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D211"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,7 +1664,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>354</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,18 +1765,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1839,7 +1824,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>325</v>
+        <v>284</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1879,114 +1864,114 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>345</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>350</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>349</v>
+        <v>306</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>351</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>341</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>338</v>
+        <v>295</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>342</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>353</v>
+        <v>310</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>352</v>
+        <v>309</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>346</v>
+        <v>303</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>347</v>
+        <v>304</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>339</v>
+        <v>296</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>343</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>340</v>
+        <v>297</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>344</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>359</v>
+        <v>316</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>360</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>361</v>
+        <v>318</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>355</v>
+        <v>312</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2351,1023 +2336,996 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>103</v>
+        <v>394</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>104</v>
+        <v>395</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>357</v>
+        <v>109</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>358</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>383</v>
+        <v>314</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>384</v>
+        <v>315</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>386</v>
+        <v>340</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>388</v>
+        <v>342</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>148</v>
-      </c>
-      <c r="B95" t="s">
-        <v>146</v>
+        <v>343</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>149</v>
-      </c>
-      <c r="B96" t="s">
-        <v>156</v>
+        <v>408</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B97" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B98" t="s">
-        <v>313</v>
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>152</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>331</v>
+        <v>150</v>
+      </c>
+      <c r="B99" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B100" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>332</v>
+        <v>289</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>155</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+      <c r="B102" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>158</v>
-      </c>
-      <c r="B103" t="s">
-        <v>159</v>
+        <v>154</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>162</v>
-      </c>
-      <c r="B104" t="s">
-        <v>163</v>
+        <v>155</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B105" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>166</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
+      </c>
+      <c r="B106" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B107" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>170</v>
-      </c>
-      <c r="B108" t="s">
-        <v>370</v>
+        <v>166</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>320</v>
+        <v>168</v>
       </c>
       <c r="B109" t="s">
-        <v>281</v>
+        <v>169</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>321</v>
+        <v>170</v>
       </c>
       <c r="B110" t="s">
-        <v>171</v>
+        <v>326</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>280</v>
       </c>
       <c r="B111" t="s">
-        <v>173</v>
+        <v>255</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B112" t="s">
-        <v>283</v>
+        <v>171</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B113" t="s">
-        <v>367</v>
+        <v>173</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>175</v>
+        <v>256</v>
       </c>
       <c r="B114" t="s">
-        <v>368</v>
+        <v>257</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>366</v>
+        <v>174</v>
       </c>
       <c r="B115" t="s">
-        <v>369</v>
+        <v>323</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>371</v>
+        <v>175</v>
       </c>
       <c r="B116" t="s">
-        <v>372</v>
+        <v>324</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>373</v>
+        <v>322</v>
       </c>
       <c r="B117" t="s">
-        <v>376</v>
+        <v>325</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>374</v>
+        <v>327</v>
       </c>
       <c r="B118" t="s">
-        <v>377</v>
+        <v>328</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>375</v>
+        <v>329</v>
       </c>
       <c r="B119" t="s">
-        <v>378</v>
+        <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>176</v>
+        <v>330</v>
       </c>
       <c r="B120" t="s">
-        <v>380</v>
+        <v>333</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>177</v>
+        <v>331</v>
       </c>
       <c r="B121" t="s">
-        <v>381</v>
+        <v>334</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>379</v>
+        <v>176</v>
       </c>
       <c r="B122" t="s">
-        <v>382</v>
+        <v>336</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B123" t="s">
-        <v>180</v>
+        <v>337</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>179</v>
+        <v>335</v>
       </c>
       <c r="B124" t="s">
-        <v>181</v>
+        <v>338</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>182</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
+      </c>
+      <c r="B125" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B126" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>185</v>
-      </c>
-      <c r="B127" t="s">
-        <v>188</v>
+        <v>182</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B128" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>389</v>
+        <v>185</v>
       </c>
       <c r="B129" t="s">
-        <v>390</v>
+        <v>188</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>391</v>
+        <v>186</v>
       </c>
       <c r="B130" t="s">
-        <v>395</v>
+        <v>189</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>392</v>
+        <v>345</v>
       </c>
       <c r="B131" t="s">
-        <v>393</v>
+        <v>346</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>394</v>
+        <v>347</v>
       </c>
       <c r="B132" t="s">
-        <v>396</v>
+        <v>351</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>190</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>397</v>
+        <v>348</v>
+      </c>
+      <c r="B133" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="B134" t="s">
-        <v>398</v>
+        <v>352</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>192</v>
-      </c>
-      <c r="B135" t="s">
-        <v>399</v>
+        <v>190</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>400</v>
+        <v>191</v>
       </c>
       <c r="B136" t="s">
-        <v>403</v>
+        <v>354</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>401</v>
+        <v>192</v>
       </c>
       <c r="B137" t="s">
-        <v>404</v>
+        <v>355</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>402</v>
+        <v>356</v>
       </c>
       <c r="B138" t="s">
-        <v>405</v>
+        <v>359</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>406</v>
+        <v>357</v>
       </c>
       <c r="B139" t="s">
-        <v>409</v>
+        <v>360</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>407</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>410</v>
+        <v>358</v>
+      </c>
+      <c r="B140" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>408</v>
+        <v>362</v>
       </c>
       <c r="B141" t="s">
-        <v>411</v>
+        <v>365</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>412</v>
-      </c>
-      <c r="B142" t="s">
-        <v>422</v>
+        <v>363</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>413</v>
+        <v>364</v>
       </c>
       <c r="B143" t="s">
-        <v>423</v>
+        <v>367</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="B144" t="s">
-        <v>415</v>
+        <v>378</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>416</v>
+        <v>369</v>
       </c>
       <c r="B145" t="s">
-        <v>419</v>
+        <v>379</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>417</v>
+        <v>370</v>
       </c>
       <c r="B146" t="s">
-        <v>420</v>
+        <v>371</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>418</v>
+        <v>372</v>
       </c>
       <c r="B147" t="s">
-        <v>421</v>
+        <v>375</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>326</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C148">
-        <v>5</v>
+        <v>373</v>
+      </c>
+      <c r="B148" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>193</v>
+        <v>374</v>
       </c>
       <c r="B149" t="s">
-        <v>201</v>
+        <v>377</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>194</v>
-      </c>
-      <c r="B150" t="s">
-        <v>195</v>
+        <v>285</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C150">
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>363</v>
+        <v>193</v>
       </c>
       <c r="B151" t="s">
-        <v>333</v>
+        <v>390</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>364</v>
-      </c>
-      <c r="B152" t="s">
-        <v>334</v>
+        <v>194</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>365</v>
-      </c>
-      <c r="B153" t="s">
-        <v>335</v>
+        <v>320</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>297</v>
-      </c>
-      <c r="B154" t="s">
-        <v>295</v>
+        <v>321</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>298</v>
-      </c>
-      <c r="B155" t="s">
-        <v>309</v>
+        <v>195</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>299</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>296</v>
+        <v>196</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B157" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>293</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>302</v>
+        <v>198</v>
+      </c>
+      <c r="B158" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>294</v>
-      </c>
-      <c r="B159" t="s">
-        <v>310</v>
+        <v>396</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>300</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>303</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>305</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>306</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>197</v>
-      </c>
-      <c r="B164" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>198</v>
-      </c>
-      <c r="B165" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>412</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>410</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>411</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>199</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>322</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="C167">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="B169" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B168" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>201</v>
+      </c>
+      <c r="B170" t="s">
         <v>203</v>
       </c>
-      <c r="B169" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>204</v>
-      </c>
-      <c r="B170" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>207</v>
+        <v>380</v>
       </c>
       <c r="B171" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>208</v>
+        <v>381</v>
       </c>
       <c r="B172" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>209</v>
-      </c>
-      <c r="B173" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>213</v>
+        <v>383</v>
       </c>
       <c r="B174" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>214</v>
+        <v>384</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>215</v>
+        <v>385</v>
       </c>
       <c r="B176" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>217</v>
-      </c>
-      <c r="B177" t="s">
-        <v>319</v>
+        <v>386</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>218</v>
-      </c>
-      <c r="B178" t="s">
-        <v>222</v>
+        <v>387</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>219</v>
-      </c>
-      <c r="B179" t="s">
-        <v>223</v>
+        <v>388</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>220</v>
-      </c>
-      <c r="B180" t="s">
-        <v>224</v>
+        <v>389</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>221</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>225</v>
+        <v>204</v>
+      </c>
+      <c r="B181" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>226</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>228</v>
+        <v>205</v>
+      </c>
+      <c r="B182" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="B183" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>230</v>
-      </c>
-      <c r="B184" t="s">
-        <v>233</v>
+        <v>282</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C184">
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>231</v>
-      </c>
-      <c r="B185" t="s">
-        <v>234</v>
+        <v>210</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="B186" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>323</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="C187">
-        <v>10</v>
+        <v>214</v>
+      </c>
+      <c r="B187" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>237</v>
-      </c>
-      <c r="B189" t="s">
-        <v>239</v>
+        <v>218</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>240</v>
-      </c>
-      <c r="B190" t="s">
-        <v>242</v>
+        <v>220</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>251</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>253</v>
+        <v>283</v>
+      </c>
+      <c r="B196" t="s">
+        <v>288</v>
+      </c>
+      <c r="C196">
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>254</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>256</v>
+        <v>232</v>
+      </c>
+      <c r="B197" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>255</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>257</v>
+        <v>233</v>
+      </c>
+      <c r="B198" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>324</v>
+        <v>236</v>
       </c>
       <c r="B199" t="s">
-        <v>330</v>
-      </c>
-      <c r="C199">
-        <v>10</v>
+        <v>239</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
+        <v>237</v>
+      </c>
+      <c r="B200" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="B200" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>259</v>
-      </c>
-      <c r="B201" t="s">
-        <v>261</v>
+        <v>238</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>262</v>
-      </c>
-      <c r="B202" t="s">
-        <v>265</v>
+        <v>241</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>284</v>
+        <v>245</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>267</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>270</v>
+        <v>252</v>
+      </c>
+      <c r="B205" t="s">
+        <v>254</v>
+      </c>
+      <c r="C205">
+        <v>3</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>268</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>271</v>
+        <v>247</v>
+      </c>
+      <c r="B206" t="s">
+        <v>253</v>
+      </c>
+      <c r="C206">
+        <v>8</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>272</v>
+        <v>249</v>
+      </c>
+      <c r="C207">
+        <v>5</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>278</v>
-      </c>
-      <c r="B208" t="s">
-        <v>280</v>
-      </c>
-      <c r="C208">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>273</v>
-      </c>
-      <c r="B209" t="s">
-        <v>279</v>
-      </c>
-      <c r="C209">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>274</v>
-      </c>
-      <c r="B210" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C210">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>276</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>277</v>
+        <v>250</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overworld 3 and colony 3 lesson stuff revised
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB718DC-5647-461C-B140-5C5DB8980243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8769D7AA-84BF-4D9F-86B3-820368697BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42225" yWindow="1485" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="398">
   <si>
     <t>Key</t>
   </si>
@@ -631,27 +631,6 @@
     <t>Our next batch of frogs are looking for a warm place with low humidity, and some nice breeze.</t>
   </si>
   <si>
-    <t>In that case, we should look for a desert climate!</t>
-  </si>
-  <si>
-    <t>overworld_3_investigate_0</t>
-  </si>
-  <si>
-    <t>overworld_3_investigate_1</t>
-  </si>
-  <si>
-    <t>overworld_3_investigate_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Now it may seem that these frogs would want to bask in the sun all day long. </t>
-  </si>
-  <si>
-    <t>However, they will still need some water source to sustain themselves!</t>
-  </si>
-  <si>
-    <t>Look for a suitable place where there are underground waters that we can extract.</t>
-  </si>
-  <si>
     <t>colony_3_intro_0</t>
   </si>
   <si>
@@ -664,36 +643,6 @@
     <t>Fortunately, there are underground waters we can extract from to make this land more habitable.</t>
   </si>
   <si>
-    <t>colony_3_water_0</t>
-  </si>
-  <si>
-    <t>colony_3_water_1</t>
-  </si>
-  <si>
-    <t>Since the ground here is not ideal for growing plants, we will have to do a bit of landscaping.</t>
-  </si>
-  <si>
-    <t>First, we will need to build a water tank where water is accessible.</t>
-  </si>
-  <si>
-    <t>colony_3_landscaping_0</t>
-  </si>
-  <si>
-    <t>Now that we have a water source, summon a landscaper to irrigate the land.</t>
-  </si>
-  <si>
-    <t>colony_3_landscaping_complete_0</t>
-  </si>
-  <si>
-    <t>colony_3_landscaping_complete_1</t>
-  </si>
-  <si>
-    <t>Excellent! Now that there’s an irrigated land, you can now place a plant on it. Do this now.</t>
-  </si>
-  <si>
-    <t>We can proceed onward once we have increased the population.</t>
-  </si>
-  <si>
     <t>overworld_4_intro_0</t>
   </si>
   <si>
@@ -706,18 +655,6 @@
     <t>Why don’t we look for a spot in the mountainous area.</t>
   </si>
   <si>
-    <t>overworld_4_investigate_0</t>
-  </si>
-  <si>
-    <t>overworld_4_investigate_1</t>
-  </si>
-  <si>
-    <t>Although we are in an area that is mostly a tropical climate, remember that altitude can also affect the climate.</t>
-  </si>
-  <si>
-    <t>Go further up where the air pressure and temperature are lower.</t>
-  </si>
-  <si>
     <t>colony_4_intro_0</t>
   </si>
   <si>
@@ -829,30 +766,9 @@
     <t>Let’s take a look again on the map.</t>
   </si>
   <si>
-    <t>These are the general directions of the global winds. As warm air from the equator rises up, it cools down and sinks towards north or south.</t>
-  </si>
-  <si>
-    <t>Sometimes, interactions between the low- and high-pressure winds will cause a cyclone, such as the ones you see on the map.</t>
-  </si>
-  <si>
-    <t>One other thing to note is how the wind drives the surface ocean currents, which help regulates the temperature across the lands.</t>
-  </si>
-  <si>
-    <t>Here is an example of an ocean current that brings warm water from the equator towards north, known as the Gulf Stream.</t>
-  </si>
-  <si>
-    <t>The Gulf Stream’s warm waters maintain a relatively warm temperature in the nearby lands throughout the year.</t>
-  </si>
-  <si>
     <t>Since Earth spins from west to east, the winds in the northern hemisphere blow northwest to southeast, and vice-versa in the southern hemisphere.</t>
   </si>
   <si>
-    <t>These cyclones can become dangerous as it accumulates wind speed and heavy amounts of water, as it travels across the land.</t>
-  </si>
-  <si>
-    <t>These are often called hurricanes in the Atlantic Ocean, and typhoons in the Pacific Ocean.</t>
-  </si>
-  <si>
     <t>It looks like they have been exiled from their planet and are looking for a new home.</t>
   </si>
   <si>
@@ -868,12 +784,6 @@
     <t>overworld_1_temp_intro_0</t>
   </si>
   <si>
-    <t>overworld_3_hint</t>
-  </si>
-  <si>
-    <t>overworld_4_hint</t>
-  </si>
-  <si>
     <t>A new house is available! Place it to increase the population!</t>
   </si>
   <si>
@@ -883,12 +793,6 @@
     <t>Press this button if you want to speed up the game.</t>
   </si>
   <si>
-    <t>Northern Africa is a good desert region for these frogs. Just make sure to pick a season that’s not too hot!</t>
-  </si>
-  <si>
-    <t>We want a mountainous area for this one. How about in South America during summer, when it is cool?</t>
-  </si>
-  <si>
     <t>Well, we can’t just let them hang about in outer space. Besides, it’s not often we are visited by space frogs!</t>
   </si>
   <si>
@@ -1177,21 +1081,6 @@
     <t>overworld_3_wind_1</t>
   </si>
   <si>
-    <t>overworld_3_wind_2</t>
-  </si>
-  <si>
-    <t>overworld_3_wind_3</t>
-  </si>
-  <si>
-    <t>overworld_3_ocean_0</t>
-  </si>
-  <si>
-    <t>overworld_3_gulf_stream_0</t>
-  </si>
-  <si>
-    <t>overworld_3_gulf_stream_1</t>
-  </si>
-  <si>
     <t>Our next batch of frogs are keen on living in a hot and humid environment.</t>
   </si>
   <si>
@@ -1274,6 +1163,57 @@
   </si>
   <si>
     <t>Though the storm may have weakened, it is still strong enough to cause wanton destruction along its path!</t>
+  </si>
+  <si>
+    <t>This time around we have wind strength as part of the criteria.</t>
+  </si>
+  <si>
+    <t>These are the general directions of the global winds.</t>
+  </si>
+  <si>
+    <t>As warm air from the equator rises up, it cools down and sinks towards north or south.</t>
+  </si>
+  <si>
+    <t>overworld_3_intro_end_0</t>
+  </si>
+  <si>
+    <t>Now with all that said and done, it’s time to find these frogs their home!</t>
+  </si>
+  <si>
+    <t>structure_fire_fight</t>
+  </si>
+  <si>
+    <t>Dousing the Flames</t>
+  </si>
+  <si>
+    <t>colony_3_flame_0</t>
+  </si>
+  <si>
+    <t>colony_3_flame_1</t>
+  </si>
+  <si>
+    <t>colony_3_flame_douse_0</t>
+  </si>
+  <si>
+    <t>colony_3_flame_douse_1</t>
+  </si>
+  <si>
+    <t>colony_3_flame_douse_2</t>
+  </si>
+  <si>
+    <t>Uh oh, one of the buildings is on fire!</t>
+  </si>
+  <si>
+    <t>Fortunately, we can extract water from our storage to douse the flames.</t>
+  </si>
+  <si>
+    <t>Due to low humidity, any flammable materials outside this dry sweltering heat can easily catch on fire.</t>
+  </si>
+  <si>
+    <t>Simply press on one of the storages, move the water on top of the flames, and then press to release the water.</t>
+  </si>
+  <si>
+    <t>Do it quickly, before the fire grows any larger!</t>
   </si>
 </sst>
 </file>
@@ -1623,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D208"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B164" sqref="B164"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,7 +1604,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1765,18 +1705,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1824,7 +1764,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1864,114 +1804,114 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>308</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>299</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>310</v>
+        <v>278</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>318</v>
+        <v>286</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>319</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2336,10 +2276,10 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>394</v>
+        <v>357</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>395</v>
+        <v>358</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2376,956 +2316,870 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>343</v>
+        <v>311</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>344</v>
+        <v>312</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>408</v>
+        <v>371</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>409</v>
+        <v>372</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>148</v>
-      </c>
-      <c r="B97" t="s">
-        <v>146</v>
+        <v>386</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B98" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B99" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B100" t="s">
-        <v>277</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>152</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>289</v>
+        <v>151</v>
+      </c>
+      <c r="B101" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>153</v>
-      </c>
-      <c r="B102" t="s">
-        <v>278</v>
+        <v>152</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>154</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>290</v>
+        <v>153</v>
+      </c>
+      <c r="B103" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>157</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>158</v>
-      </c>
-      <c r="B105" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B106" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B107" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>166</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B108" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>168</v>
-      </c>
-      <c r="B109" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B110" t="s">
-        <v>326</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>280</v>
+        <v>170</v>
       </c>
       <c r="B111" t="s">
-        <v>255</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>281</v>
+        <v>252</v>
       </c>
       <c r="B112" t="s">
-        <v>171</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>172</v>
+        <v>253</v>
       </c>
       <c r="B113" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>256</v>
+        <v>172</v>
       </c>
       <c r="B114" t="s">
-        <v>257</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>174</v>
+        <v>235</v>
       </c>
       <c r="B115" t="s">
-        <v>323</v>
+        <v>236</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B116" t="s">
-        <v>324</v>
+        <v>291</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>322</v>
+        <v>175</v>
       </c>
       <c r="B117" t="s">
-        <v>325</v>
+        <v>292</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>327</v>
+        <v>290</v>
       </c>
       <c r="B118" t="s">
-        <v>328</v>
+        <v>293</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>329</v>
+        <v>295</v>
       </c>
       <c r="B119" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>330</v>
+        <v>297</v>
       </c>
       <c r="B120" t="s">
-        <v>333</v>
+        <v>300</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>331</v>
+        <v>298</v>
       </c>
       <c r="B121" t="s">
-        <v>334</v>
+        <v>301</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>176</v>
+        <v>299</v>
       </c>
       <c r="B122" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>337</v>
+        <v>304</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>335</v>
+        <v>177</v>
       </c>
       <c r="B124" t="s">
-        <v>338</v>
+        <v>305</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>178</v>
+        <v>303</v>
       </c>
       <c r="B125" t="s">
-        <v>180</v>
+        <v>306</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B126" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>182</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
+      </c>
+      <c r="B127" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>184</v>
-      </c>
-      <c r="B128" t="s">
-        <v>187</v>
+        <v>182</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B129" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B130" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>345</v>
+        <v>186</v>
       </c>
       <c r="B131" t="s">
-        <v>346</v>
+        <v>189</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>347</v>
+        <v>313</v>
       </c>
       <c r="B132" t="s">
-        <v>351</v>
+        <v>314</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>348</v>
+        <v>315</v>
       </c>
       <c r="B133" t="s">
-        <v>349</v>
+        <v>319</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>350</v>
+        <v>316</v>
       </c>
       <c r="B134" t="s">
-        <v>352</v>
+        <v>317</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>190</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>353</v>
+        <v>318</v>
+      </c>
+      <c r="B135" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>191</v>
-      </c>
-      <c r="B136" t="s">
-        <v>354</v>
+        <v>190</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B137" t="s">
-        <v>355</v>
+        <v>322</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>356</v>
+        <v>192</v>
       </c>
       <c r="B138" t="s">
-        <v>359</v>
+        <v>323</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>357</v>
+        <v>324</v>
       </c>
       <c r="B139" t="s">
-        <v>360</v>
+        <v>327</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>358</v>
+        <v>325</v>
       </c>
       <c r="B140" t="s">
-        <v>361</v>
+        <v>328</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>362</v>
+        <v>326</v>
       </c>
       <c r="B141" t="s">
-        <v>365</v>
+        <v>329</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>363</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>366</v>
+        <v>330</v>
+      </c>
+      <c r="B142" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>364</v>
-      </c>
-      <c r="B143" t="s">
-        <v>367</v>
+        <v>331</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>368</v>
+        <v>332</v>
       </c>
       <c r="B144" t="s">
-        <v>378</v>
+        <v>335</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>369</v>
+        <v>336</v>
       </c>
       <c r="B145" t="s">
-        <v>379</v>
+        <v>346</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>370</v>
+        <v>337</v>
       </c>
       <c r="B146" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>372</v>
+        <v>338</v>
       </c>
       <c r="B147" t="s">
-        <v>375</v>
+        <v>339</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>373</v>
+        <v>340</v>
       </c>
       <c r="B148" t="s">
-        <v>376</v>
+        <v>343</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>374</v>
+        <v>341</v>
       </c>
       <c r="B149" t="s">
-        <v>377</v>
+        <v>344</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>285</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C150">
-        <v>5</v>
+        <v>342</v>
+      </c>
+      <c r="B150" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>193</v>
-      </c>
-      <c r="B151" t="s">
-        <v>390</v>
+        <v>255</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C151">
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>194</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>391</v>
+        <v>193</v>
+      </c>
+      <c r="B152" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>320</v>
-      </c>
-      <c r="B153" s="5" t="s">
-        <v>291</v>
+        <v>194</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>321</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>195</v>
+        <v>289</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>392</v>
+        <v>260</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>393</v>
+        <v>355</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>197</v>
-      </c>
-      <c r="B157" t="s">
-        <v>279</v>
+        <v>196</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B158" t="s">
-        <v>199</v>
+        <v>251</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>396</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>397</v>
+        <v>198</v>
+      </c>
+      <c r="B159" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>398</v>
+        <v>359</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>400</v>
+        <v>360</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>399</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>401</v>
+        <v>361</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>402</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>404</v>
+        <v>362</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>403</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>416</v>
+        <v>365</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>405</v>
+        <v>366</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>407</v>
+        <v>379</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>406</v>
+        <v>368</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>417</v>
+        <v>370</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>412</v>
+        <v>369</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>413</v>
+        <v>380</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>410</v>
+        <v>375</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>414</v>
+        <v>376</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>411</v>
-      </c>
-      <c r="B168" s="5" t="s">
-        <v>415</v>
+        <v>373</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>200</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>202</v>
+        <v>374</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>201</v>
-      </c>
-      <c r="B170" t="s">
-        <v>203</v>
+        <v>200</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>380</v>
-      </c>
-      <c r="B171" t="s">
-        <v>267</v>
+        <v>201</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>381</v>
+        <v>348</v>
       </c>
       <c r="B172" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>382</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>268</v>
+        <v>349</v>
+      </c>
+      <c r="B173" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>383</v>
-      </c>
-      <c r="B174" t="s">
-        <v>269</v>
+        <v>350</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>384</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>270</v>
+        <v>351</v>
+      </c>
+      <c r="B175" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>352</v>
+      </c>
+      <c r="B176" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>384</v>
+      </c>
+      <c r="B177" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="B176" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>386</v>
-      </c>
-      <c r="B177" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>387</v>
+        <v>203</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>204</v>
+      </c>
+      <c r="B179" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>388</v>
       </c>
-      <c r="B179" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+      <c r="B180" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>389</v>
       </c>
-      <c r="B180" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>204</v>
-      </c>
-      <c r="B181" t="s">
+      <c r="B181" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>390</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>391</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>392</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>205</v>
-      </c>
-      <c r="B182" t="s">
+      <c r="B185" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>206</v>
-      </c>
-      <c r="B183" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>282</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C184">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="B186" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B185" s="3" t="s">
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>211</v>
+      </c>
+      <c r="B187" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>211</v>
-      </c>
-      <c r="B186" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="B188" t="s">
         <v>214</v>
       </c>
-      <c r="B187" t="s">
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>215</v>
+      </c>
+      <c r="B189" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>215</v>
-      </c>
-      <c r="B188" s="3" t="s">
+      <c r="B190" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>218</v>
-      </c>
-      <c r="B189" s="3" t="s">
+      <c r="B191" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>220</v>
       </c>
-      <c r="B190" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>221</v>
-      </c>
-      <c r="B191" s="3" t="s">
+      <c r="B192" s="3" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>224</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>229</v>
-      </c>
-      <c r="B195" s="3" t="s">
         <v>231</v>
+      </c>
+      <c r="B195" t="s">
+        <v>233</v>
+      </c>
+      <c r="C195">
+        <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>283</v>
+        <v>226</v>
       </c>
       <c r="B196" t="s">
-        <v>288</v>
+        <v>232</v>
       </c>
       <c r="C196">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>232</v>
-      </c>
-      <c r="B197" t="s">
-        <v>234</v>
+        <v>227</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C197">
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>233</v>
-      </c>
-      <c r="B198" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>236</v>
-      </c>
-      <c r="B199" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>237</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>238</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>241</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>242</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>243</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>252</v>
-      </c>
-      <c r="B205" t="s">
-        <v>254</v>
-      </c>
-      <c r="C205">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>247</v>
-      </c>
-      <c r="B206" t="s">
-        <v>253</v>
-      </c>
-      <c r="C206">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>248</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C207">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>250</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>251</v>
+        <v>229</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overworld/colony 4 lesson stuff revised
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8769D7AA-84BF-4D9F-86B3-820368697BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB1BB20-2BEC-4F00-A5E2-423F55EA9790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42225" yWindow="1485" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39795" yWindow="1380" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -649,39 +649,12 @@
     <t>overworld_4_intro_1</t>
   </si>
   <si>
-    <t>This is our final batch of frogs, and they seem eager to settle in the highlands where it’s cold and snowy.</t>
-  </si>
-  <si>
-    <t>Why don’t we look for a spot in the mountainous area.</t>
-  </si>
-  <si>
     <t>colony_4_intro_0</t>
   </si>
   <si>
     <t>colony_4_intro_1</t>
   </si>
   <si>
-    <t>The highland climate is quite comfy despite the consistent cold weather. We’ll need more than usual power to keep our houses warm.</t>
-  </si>
-  <si>
-    <t>Just like in the desert climate, the ground here is not ideal for plants to grow, so landscaping will be crucial.</t>
-  </si>
-  <si>
-    <t>colony_4_landscape_0</t>
-  </si>
-  <si>
-    <t>colony_4_landscape_1</t>
-  </si>
-  <si>
-    <t>colony_4_landscape_2</t>
-  </si>
-  <si>
-    <t>Since we can’t place plants on these rigid grounds, we’ll once again need the help of landscapers to shape the land.</t>
-  </si>
-  <si>
-    <t>We will be able to proceed once the frog population has increased.</t>
-  </si>
-  <si>
     <t>colony_4_cave_0</t>
   </si>
   <si>
@@ -697,9 +670,6 @@
     <t>Critters will keep emerging from these caves so long as it remains. Fortunately, an engineer can demolish it.</t>
   </si>
   <si>
-    <t>Make sure to also have a hero frog around to deal with the critters, while the engineers do their work!</t>
-  </si>
-  <si>
     <t>end</t>
   </si>
   <si>
@@ -733,9 +703,6 @@
     <t>This is due to the earth's equator facing more directly towards the sun.</t>
   </si>
   <si>
-    <t>You won’t have to worry about where to place the water tank this time around.</t>
-  </si>
-  <si>
     <t>analyze</t>
   </si>
   <si>
@@ -1214,6 +1181,39 @@
   </si>
   <si>
     <t>Do it quickly, before the fire grows any larger!</t>
+  </si>
+  <si>
+    <t>While consistently cold places can be found at the furthest north or south of Earth, they can also be found in high altitude.</t>
+  </si>
+  <si>
+    <t>This is our final batch of frogs, and they seem eager to settle to a place where it’s cold and snowy.</t>
+  </si>
+  <si>
+    <t>The highland climate is quite comfy despite the consistent cold weather.</t>
+  </si>
+  <si>
+    <t>We’ll need more than usual power to keep our houses warm.</t>
+  </si>
+  <si>
+    <t>Make sure to also have a fighter frog around to deal with the critters, while the engineers do their work!</t>
+  </si>
+  <si>
+    <t>colony_4_storm_0</t>
+  </si>
+  <si>
+    <t>colony_4_storm_1</t>
+  </si>
+  <si>
+    <t>colony_4_storm_2</t>
+  </si>
+  <si>
+    <t>Watch out for icy boulders!</t>
+  </si>
+  <si>
+    <t>Just like storms can form from the tropics, they can also form in cold regions near large body of water.</t>
+  </si>
+  <si>
+    <t>Remember to activate the wind turbines to repel these icy assaults!</t>
   </si>
 </sst>
 </file>
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="A192" sqref="A192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1604,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1705,18 +1705,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1764,7 +1764,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1804,114 +1804,114 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2276,10 +2276,10 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2316,50 +2316,50 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2391,7 +2391,7 @@
         <v>151</v>
       </c>
       <c r="B101" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2399,7 +2399,7 @@
         <v>152</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
         <v>153</v>
       </c>
       <c r="B103" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2415,7 +2415,7 @@
         <v>154</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,20 +2471,20 @@
         <v>170</v>
       </c>
       <c r="B111" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B112" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="B113" t="s">
         <v>171</v>
@@ -2500,10 +2500,10 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B115" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,7 +2511,7 @@
         <v>174</v>
       </c>
       <c r="B116" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2519,47 +2519,47 @@
         <v>175</v>
       </c>
       <c r="B117" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B118" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B119" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B120" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B121" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B122" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,15 +2575,15 @@
         <v>177</v>
       </c>
       <c r="B124" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="B125" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2636,34 +2636,34 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="B132" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="B133" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B134" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="B135" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
         <v>190</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,7 +2679,7 @@
         <v>191</v>
       </c>
       <c r="B137" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,111 +2687,111 @@
         <v>192</v>
       </c>
       <c r="B138" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="B139" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B140" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="B141" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B142" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="B144" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="B145" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="B146" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="B147" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B148" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="B149" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="B150" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C151">
         <v>5</v>
@@ -2802,7 +2802,7 @@
         <v>193</v>
       </c>
       <c r="B152" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2810,23 +2810,23 @@
         <v>194</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2834,7 +2834,7 @@
         <v>195</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2842,7 +2842,7 @@
         <v>196</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2850,7 +2850,7 @@
         <v>197</v>
       </c>
       <c r="B158" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2863,82 +2863,82 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
+        <v>358</v>
+      </c>
+      <c r="B166" s="4" t="s">
         <v>369</v>
-      </c>
-      <c r="B166" s="4" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -2954,55 +2954,55 @@
         <v>201</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="B172" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="B173" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="B175" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="B176" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -3023,130 +3023,130 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>207</v>
       </c>
-      <c r="B185" s="3" t="s">
-        <v>209</v>
+      <c r="B185" s="4" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>208</v>
       </c>
-      <c r="B186" s="3" t="s">
-        <v>210</v>
+      <c r="B186" s="5" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B187" t="s">
-        <v>213</v>
+        <v>389</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B188" t="s">
-        <v>214</v>
+        <v>390</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>215</v>
-      </c>
-      <c r="B189" t="s">
-        <v>218</v>
+        <v>211</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>219</v>
+        <v>391</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>220</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>223</v>
+        <v>392</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>221</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>224</v>
+        <v>393</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>222</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>225</v>
+        <v>394</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B195" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C195">
         <v>3</v>
@@ -3154,10 +3154,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B196" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C196">
         <v>8</v>
@@ -3165,10 +3165,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C197">
         <v>5</v>
@@ -3176,10 +3176,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>